<commit_message>
adding send sale report on the email
</commit_message>
<xml_diff>
--- a/saleReport.xlsx
+++ b/saleReport.xlsx
@@ -1582,117 +1582,117 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3646,7 +3646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:N95"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -3668,45 +3668,45 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A4" s="101" t="s">
+      <c r="A4" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="101"/>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="101"/>
-      <c r="J4" s="101"/>
-      <c r="K4" s="101"/>
+      <c r="B4" s="107"/>
+      <c r="C4" s="107"/>
+      <c r="D4" s="107"/>
+      <c r="E4" s="107"/>
+      <c r="F4" s="107"/>
+      <c r="G4" s="107"/>
+      <c r="H4" s="107"/>
+      <c r="I4" s="107"/>
+      <c r="J4" s="107"/>
+      <c r="K4" s="107"/>
     </row>
     <row r="5" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A5" s="101"/>
-      <c r="B5" s="101"/>
-      <c r="C5" s="101"/>
-      <c r="D5" s="101"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="101"/>
-      <c r="G5" s="101"/>
-      <c r="H5" s="101"/>
-      <c r="I5" s="101"/>
-      <c r="J5" s="101"/>
-      <c r="K5" s="101"/>
+      <c r="A5" s="107"/>
+      <c r="B5" s="107"/>
+      <c r="C5" s="107"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="107"/>
+      <c r="F5" s="107"/>
+      <c r="G5" s="107"/>
+      <c r="H5" s="107"/>
+      <c r="I5" s="107"/>
+      <c r="J5" s="107"/>
+      <c r="K5" s="107"/>
     </row>
     <row r="6" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A6" s="101"/>
-      <c r="B6" s="101"/>
-      <c r="C6" s="101"/>
-      <c r="D6" s="101"/>
-      <c r="E6" s="101"/>
-      <c r="F6" s="101"/>
-      <c r="G6" s="101"/>
-      <c r="H6" s="101"/>
-      <c r="I6" s="101"/>
-      <c r="J6" s="101"/>
-      <c r="K6" s="101"/>
+      <c r="A6" s="107"/>
+      <c r="B6" s="107"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="107"/>
+      <c r="F6" s="107"/>
+      <c r="G6" s="107"/>
+      <c r="H6" s="107"/>
+      <c r="I6" s="107"/>
+      <c r="J6" s="107"/>
+      <c r="K6" s="107"/>
     </row>
     <row r="8" spans="1:12" ht="14.7" thickBot="1">
       <c r="C8" s="75"/>
@@ -3961,7 +3961,7 @@
       <c r="G23" s="94" t="s">
         <v>195</v>
       </c>
-      <c r="H23" s="136" t="s">
+      <c r="H23" s="101" t="s">
         <v>121</v>
       </c>
       <c r="I23" s="96"/>
@@ -3991,7 +3991,7 @@
       <c r="G24" s="94" t="s">
         <v>196</v>
       </c>
-      <c r="H24" s="136" t="s">
+      <c r="H24" s="101" t="s">
         <v>119</v>
       </c>
       <c r="I24" s="96"/>
@@ -4021,7 +4021,7 @@
       <c r="G25" s="94" t="s">
         <v>90</v>
       </c>
-      <c r="H25" s="136" t="s">
+      <c r="H25" s="101" t="s">
         <v>117</v>
       </c>
       <c r="I25" s="96"/>
@@ -4036,14 +4036,14 @@
       <c r="B26" s="94" t="s">
         <v>179</v>
       </c>
-      <c r="C26" s="137"/>
+      <c r="C26" s="102"/>
       <c r="D26" s="94" t="s">
         <v>165</v>
       </c>
       <c r="E26" s="94" t="s">
         <v>72</v>
       </c>
-      <c r="F26" s="137"/>
+      <c r="F26" s="102"/>
       <c r="G26" s="94" t="s">
         <v>91</v>
       </c>
@@ -4062,18 +4062,18 @@
       <c r="B27" s="94" t="s">
         <v>183</v>
       </c>
-      <c r="C27" s="137"/>
+      <c r="C27" s="102"/>
       <c r="D27" s="94" t="s">
         <v>57</v>
       </c>
       <c r="E27" s="94" t="s">
         <v>172</v>
       </c>
-      <c r="F27" s="137"/>
+      <c r="F27" s="102"/>
       <c r="G27" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="H27" s="138"/>
+      <c r="H27" s="103"/>
       <c r="I27" s="96"/>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
@@ -4086,18 +4086,18 @@
       <c r="B28" s="94" t="s">
         <v>133</v>
       </c>
-      <c r="C28" s="139"/>
+      <c r="C28" s="104"/>
       <c r="D28" s="94" t="s">
         <v>60</v>
       </c>
       <c r="E28" s="94" t="s">
         <v>173</v>
       </c>
-      <c r="F28" s="137"/>
+      <c r="F28" s="102"/>
       <c r="G28" s="94" t="s">
         <v>199</v>
       </c>
-      <c r="H28" s="138"/>
+      <c r="H28" s="103"/>
       <c r="I28" s="96"/>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
@@ -4110,16 +4110,16 @@
       <c r="B29" s="94" t="s">
         <v>132</v>
       </c>
-      <c r="C29" s="139"/>
+      <c r="C29" s="104"/>
       <c r="D29" s="94" t="s">
         <v>166</v>
       </c>
       <c r="E29" s="94" t="s">
         <v>174</v>
       </c>
-      <c r="F29" s="137"/>
-      <c r="G29" s="137"/>
-      <c r="H29" s="138"/>
+      <c r="F29" s="102"/>
+      <c r="G29" s="102"/>
+      <c r="H29" s="103"/>
       <c r="I29" s="96"/>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
@@ -4132,94 +4132,94 @@
       <c r="B30" s="94" t="s">
         <v>134</v>
       </c>
-      <c r="C30" s="139"/>
+      <c r="C30" s="104"/>
       <c r="D30" s="94" t="s">
         <v>62</v>
       </c>
       <c r="E30" s="94" t="s">
         <v>175</v>
       </c>
-      <c r="F30" s="138"/>
-      <c r="G30" s="137"/>
-      <c r="H30" s="138"/>
+      <c r="F30" s="103"/>
+      <c r="G30" s="102"/>
+      <c r="H30" s="103"/>
       <c r="I30" s="96"/>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="137"/>
+      <c r="A31" s="102"/>
       <c r="B31" s="94" t="s">
         <v>135</v>
       </c>
-      <c r="C31" s="139"/>
+      <c r="C31" s="104"/>
       <c r="D31" s="94" t="s">
         <v>167</v>
       </c>
       <c r="E31" s="94" t="s">
         <v>176</v>
       </c>
-      <c r="F31" s="138"/>
-      <c r="G31" s="137"/>
-      <c r="H31" s="138"/>
+      <c r="F31" s="103"/>
+      <c r="G31" s="102"/>
+      <c r="H31" s="103"/>
       <c r="I31" s="96"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
       <c r="L31" s="9"/>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="137"/>
+      <c r="A32" s="102"/>
       <c r="B32" s="94" t="s">
         <v>160</v>
       </c>
-      <c r="C32" s="139"/>
+      <c r="C32" s="104"/>
       <c r="D32" s="94" t="s">
         <v>168</v>
       </c>
       <c r="E32" s="94" t="s">
         <v>177</v>
       </c>
-      <c r="F32" s="138"/>
-      <c r="G32" s="137"/>
-      <c r="H32" s="138"/>
+      <c r="F32" s="103"/>
+      <c r="G32" s="102"/>
+      <c r="H32" s="103"/>
       <c r="I32" s="96"/>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
       <c r="L32" s="9"/>
     </row>
     <row r="33" spans="1:14">
-      <c r="A33" s="137"/>
+      <c r="A33" s="102"/>
       <c r="B33" s="94" t="s">
         <v>136</v>
       </c>
-      <c r="C33" s="139"/>
+      <c r="C33" s="104"/>
       <c r="D33" s="94" t="s">
         <v>65</v>
       </c>
-      <c r="E33" s="140" t="s">
+      <c r="E33" s="105" t="s">
         <v>206</v>
       </c>
-      <c r="F33" s="137"/>
-      <c r="G33" s="137"/>
-      <c r="H33" s="138"/>
+      <c r="F33" s="102"/>
+      <c r="G33" s="102"/>
+      <c r="H33" s="103"/>
       <c r="I33" s="96"/>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
       <c r="L33" s="9"/>
     </row>
     <row r="34" spans="1:14">
-      <c r="A34" s="137"/>
+      <c r="A34" s="102"/>
       <c r="B34" s="94" t="s">
         <v>137</v>
       </c>
-      <c r="C34" s="139"/>
+      <c r="C34" s="104"/>
       <c r="D34" s="94" t="s">
         <v>66</v>
       </c>
-      <c r="E34" s="141"/>
-      <c r="F34" s="137"/>
-      <c r="G34" s="137"/>
-      <c r="H34" s="138"/>
+      <c r="E34" s="106"/>
+      <c r="F34" s="102"/>
+      <c r="G34" s="102"/>
+      <c r="H34" s="103"/>
       <c r="I34" s="96"/>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
@@ -4349,35 +4349,35 @@
       <c r="N41" s="75"/>
     </row>
     <row r="42" spans="1:14" ht="25">
-      <c r="A42" s="133" t="s">
+      <c r="A42" s="139" t="s">
         <v>103</v>
       </c>
-      <c r="B42" s="134"/>
-      <c r="C42" s="134"/>
-      <c r="D42" s="135"/>
+      <c r="B42" s="140"/>
+      <c r="C42" s="140"/>
+      <c r="D42" s="141"/>
       <c r="E42" s="10"/>
-      <c r="F42" s="124" t="s">
+      <c r="F42" s="130" t="s">
         <v>103</v>
       </c>
-      <c r="G42" s="125"/>
-      <c r="H42" s="125"/>
-      <c r="I42" s="126"/>
+      <c r="G42" s="131"/>
+      <c r="H42" s="131"/>
+      <c r="I42" s="132"/>
       <c r="K42" s="5"/>
     </row>
     <row r="43" spans="1:14" ht="20.350000000000001" thickBot="1">
-      <c r="A43" s="130" t="s">
+      <c r="A43" s="136" t="s">
         <v>9</v>
       </c>
-      <c r="B43" s="131"/>
-      <c r="C43" s="131"/>
-      <c r="D43" s="132"/>
+      <c r="B43" s="137"/>
+      <c r="C43" s="137"/>
+      <c r="D43" s="138"/>
       <c r="E43" s="8"/>
-      <c r="F43" s="127" t="s">
+      <c r="F43" s="133" t="s">
         <v>13</v>
       </c>
-      <c r="G43" s="128"/>
-      <c r="H43" s="128"/>
-      <c r="I43" s="129"/>
+      <c r="G43" s="134"/>
+      <c r="H43" s="134"/>
+      <c r="I43" s="135"/>
     </row>
     <row r="44" spans="1:14" s="1" customFormat="1" ht="49.5" customHeight="1" thickBot="1">
       <c r="A44" s="11" t="s">
@@ -4470,32 +4470,32 @@
       <c r="K50" s="8"/>
     </row>
     <row r="51" spans="1:13" ht="17.7" thickBot="1">
-      <c r="A51" s="121"/>
-      <c r="B51" s="122"/>
-      <c r="C51" s="122"/>
-      <c r="D51" s="122"/>
-      <c r="E51" s="122"/>
-      <c r="F51" s="122"/>
-      <c r="G51" s="122"/>
-      <c r="H51" s="122"/>
-      <c r="I51" s="122"/>
-      <c r="J51" s="122"/>
-      <c r="K51" s="123"/>
+      <c r="A51" s="127"/>
+      <c r="B51" s="128"/>
+      <c r="C51" s="128"/>
+      <c r="D51" s="128"/>
+      <c r="E51" s="128"/>
+      <c r="F51" s="128"/>
+      <c r="G51" s="128"/>
+      <c r="H51" s="128"/>
+      <c r="I51" s="128"/>
+      <c r="J51" s="128"/>
+      <c r="K51" s="129"/>
     </row>
     <row r="53" spans="1:13" ht="27.7">
-      <c r="A53" s="113" t="s">
+      <c r="A53" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="B53" s="113"/>
-      <c r="C53" s="113"/>
-      <c r="D53" s="113"/>
-      <c r="E53" s="113"/>
-      <c r="F53" s="113"/>
-      <c r="G53" s="113"/>
-      <c r="H53" s="113"/>
-      <c r="I53" s="113"/>
-      <c r="J53" s="113"/>
-      <c r="K53" s="113"/>
+      <c r="B53" s="119"/>
+      <c r="C53" s="119"/>
+      <c r="D53" s="119"/>
+      <c r="E53" s="119"/>
+      <c r="F53" s="119"/>
+      <c r="G53" s="119"/>
+      <c r="H53" s="119"/>
+      <c r="I53" s="119"/>
+      <c r="J53" s="119"/>
+      <c r="K53" s="119"/>
     </row>
     <row r="55" spans="1:13" ht="20">
       <c r="A55" s="43" t="s">
@@ -4907,21 +4907,21 @@
       <c r="J82" s="8"/>
     </row>
     <row r="83" spans="1:12" ht="17.7" thickBot="1">
-      <c r="A83" s="102" t="s">
+      <c r="A83" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="B83" s="114"/>
-      <c r="C83" s="103"/>
+      <c r="B83" s="120"/>
+      <c r="C83" s="109"/>
       <c r="D83" s="65">
         <f>SUM($D$58:$D$81)</f>
         <v>0</v>
       </c>
       <c r="E83" s="15"/>
       <c r="F83" s="15"/>
-      <c r="G83" s="102" t="s">
+      <c r="G83" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="H83" s="103"/>
+      <c r="H83" s="109"/>
       <c r="I83" s="65">
         <f>SUM(I58:I81)</f>
         <v>0</v>
@@ -4929,11 +4929,11 @@
       <c r="J83" s="8"/>
     </row>
     <row r="84" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A84" s="118" t="s">
+      <c r="A84" s="124" t="s">
         <v>147</v>
       </c>
-      <c r="B84" s="119"/>
-      <c r="C84" s="120"/>
+      <c r="B84" s="125"/>
+      <c r="C84" s="126"/>
       <c r="D84" s="78">
         <f>SUMIF($B$58:$B$81,גיליון2!$D$2,גיליון1!$D$58:$D$81)</f>
         <v>0</v>
@@ -4946,11 +4946,11 @@
       <c r="J84" s="8"/>
     </row>
     <row r="85" spans="1:12" ht="14.7" thickBot="1">
-      <c r="A85" s="115" t="s">
+      <c r="A85" s="121" t="s">
         <v>148</v>
       </c>
-      <c r="B85" s="116"/>
-      <c r="C85" s="117"/>
+      <c r="B85" s="122"/>
+      <c r="C85" s="123"/>
       <c r="D85" s="78">
         <f>SUMIF($B$58:$B$81,גיליון2!$D$3,גיליון1!$D$58:$D$81)</f>
         <v>0</v>
@@ -4963,11 +4963,11 @@
       <c r="J85" s="8"/>
     </row>
     <row r="86" spans="1:12" ht="17.7" thickBot="1">
-      <c r="A86" s="102" t="s">
+      <c r="A86" s="108" t="s">
         <v>144</v>
       </c>
-      <c r="B86" s="114"/>
-      <c r="C86" s="103"/>
+      <c r="B86" s="120"/>
+      <c r="C86" s="109"/>
       <c r="D86" s="65">
         <f>$D$83-$D$84-$D$85</f>
         <v>0</v>
@@ -5024,74 +5024,74 @@
       <c r="L89" s="8"/>
     </row>
     <row r="90" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A90" s="104"/>
-      <c r="B90" s="105"/>
-      <c r="C90" s="105"/>
-      <c r="D90" s="105"/>
-      <c r="E90" s="105"/>
-      <c r="F90" s="105"/>
-      <c r="G90" s="105"/>
-      <c r="H90" s="105"/>
-      <c r="I90" s="105"/>
-      <c r="J90" s="105"/>
-      <c r="K90" s="105"/>
-      <c r="L90" s="106"/>
+      <c r="A90" s="110"/>
+      <c r="B90" s="111"/>
+      <c r="C90" s="111"/>
+      <c r="D90" s="111"/>
+      <c r="E90" s="111"/>
+      <c r="F90" s="111"/>
+      <c r="G90" s="111"/>
+      <c r="H90" s="111"/>
+      <c r="I90" s="111"/>
+      <c r="J90" s="111"/>
+      <c r="K90" s="111"/>
+      <c r="L90" s="112"/>
     </row>
     <row r="91" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A91" s="107"/>
-      <c r="B91" s="108"/>
-      <c r="C91" s="108"/>
-      <c r="D91" s="108"/>
-      <c r="E91" s="108"/>
-      <c r="F91" s="108"/>
-      <c r="G91" s="108"/>
-      <c r="H91" s="108"/>
-      <c r="I91" s="108"/>
-      <c r="J91" s="108"/>
-      <c r="K91" s="108"/>
-      <c r="L91" s="109"/>
+      <c r="A91" s="113"/>
+      <c r="B91" s="114"/>
+      <c r="C91" s="114"/>
+      <c r="D91" s="114"/>
+      <c r="E91" s="114"/>
+      <c r="F91" s="114"/>
+      <c r="G91" s="114"/>
+      <c r="H91" s="114"/>
+      <c r="I91" s="114"/>
+      <c r="J91" s="114"/>
+      <c r="K91" s="114"/>
+      <c r="L91" s="115"/>
     </row>
     <row r="92" spans="1:12">
-      <c r="A92" s="107"/>
-      <c r="B92" s="108"/>
-      <c r="C92" s="108"/>
-      <c r="D92" s="108"/>
-      <c r="E92" s="108"/>
-      <c r="F92" s="108"/>
-      <c r="G92" s="108"/>
-      <c r="H92" s="108"/>
-      <c r="I92" s="108"/>
-      <c r="J92" s="108"/>
-      <c r="K92" s="108"/>
-      <c r="L92" s="109"/>
+      <c r="A92" s="113"/>
+      <c r="B92" s="114"/>
+      <c r="C92" s="114"/>
+      <c r="D92" s="114"/>
+      <c r="E92" s="114"/>
+      <c r="F92" s="114"/>
+      <c r="G92" s="114"/>
+      <c r="H92" s="114"/>
+      <c r="I92" s="114"/>
+      <c r="J92" s="114"/>
+      <c r="K92" s="114"/>
+      <c r="L92" s="115"/>
     </row>
     <row r="93" spans="1:12">
-      <c r="A93" s="107"/>
-      <c r="B93" s="108"/>
-      <c r="C93" s="108"/>
-      <c r="D93" s="108"/>
-      <c r="E93" s="108"/>
-      <c r="F93" s="108"/>
-      <c r="G93" s="108"/>
-      <c r="H93" s="108"/>
-      <c r="I93" s="108"/>
-      <c r="J93" s="108"/>
-      <c r="K93" s="108"/>
-      <c r="L93" s="109"/>
+      <c r="A93" s="113"/>
+      <c r="B93" s="114"/>
+      <c r="C93" s="114"/>
+      <c r="D93" s="114"/>
+      <c r="E93" s="114"/>
+      <c r="F93" s="114"/>
+      <c r="G93" s="114"/>
+      <c r="H93" s="114"/>
+      <c r="I93" s="114"/>
+      <c r="J93" s="114"/>
+      <c r="K93" s="114"/>
+      <c r="L93" s="115"/>
     </row>
     <row r="94" spans="1:12">
-      <c r="A94" s="110"/>
-      <c r="B94" s="111"/>
-      <c r="C94" s="111"/>
-      <c r="D94" s="111"/>
-      <c r="E94" s="111"/>
-      <c r="F94" s="111"/>
-      <c r="G94" s="111"/>
-      <c r="H94" s="111"/>
-      <c r="I94" s="111"/>
-      <c r="J94" s="111"/>
-      <c r="K94" s="111"/>
-      <c r="L94" s="112"/>
+      <c r="A94" s="116"/>
+      <c r="B94" s="117"/>
+      <c r="C94" s="117"/>
+      <c r="D94" s="117"/>
+      <c r="E94" s="117"/>
+      <c r="F94" s="117"/>
+      <c r="G94" s="117"/>
+      <c r="H94" s="117"/>
+      <c r="I94" s="117"/>
+      <c r="J94" s="117"/>
+      <c r="K94" s="117"/>
+      <c r="L94" s="118"/>
     </row>
     <row r="95" spans="1:12">
       <c r="A95" s="8"/>

</xml_diff>

<commit_message>
fixing issue in the sale report xl
</commit_message>
<xml_diff>
--- a/saleReport.xlsx
+++ b/saleReport.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\matan\לימודים\final project\SE-projrct\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\matan\לימודים\SE-prorject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,31 +13,30 @@
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
-    <sheet name="גיליון2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="FEVER_TREE">גיליון2!$A$10</definedName>
-    <definedName name="LIMITED_EDITION">גיליון2!$X$2:$X$5</definedName>
-    <definedName name="אדמה">גיליון2!$S$2:$S$9</definedName>
-    <definedName name="אדמה_2_חדשה">גיליון2!$AC$2:$AC$8</definedName>
-    <definedName name="אדמה_בלנד">גיליון2!$U$2:$U$5</definedName>
-    <definedName name="אפרטיף">גיליון2!$N$2:$N$13</definedName>
-    <definedName name="גין">גיליון2!$J$2:$J$5</definedName>
-    <definedName name="הר">גיליון2!$Q$2:$Q$6</definedName>
-    <definedName name="וודקה">גיליון2!$F$2:$F$9</definedName>
-    <definedName name="וויסקי">גיליון2!$D$2:$D$59</definedName>
-    <definedName name="טקילה">גיליון2!$L$2:$L$4</definedName>
-    <definedName name="יין_מבעבע_צינזאנו">גיליון2!$AA$2:$AA$6</definedName>
-    <definedName name="ליקרים_דזסטיף">גיליון2!$O$2:$O$7</definedName>
-    <definedName name="פנינים">גיליון2!$Z$2:$Z$4</definedName>
-    <definedName name="רום">גיליון2!$H$2:$H$7</definedName>
+    <definedName name="FEVER_TREE">#REF!</definedName>
+    <definedName name="LIMITED_EDITION">#REF!</definedName>
+    <definedName name="אדמה">#REF!</definedName>
+    <definedName name="אדמה_2_חדשה">#REF!</definedName>
+    <definedName name="אדמה_בלנד">#REF!</definedName>
+    <definedName name="אפרטיף">#REF!</definedName>
+    <definedName name="גין">#REF!</definedName>
+    <definedName name="הר">#REF!</definedName>
+    <definedName name="וודקה">#REF!</definedName>
+    <definedName name="וויסקי">#REF!</definedName>
+    <definedName name="טקילה">#REF!</definedName>
+    <definedName name="יין_מבעבע_צינזאנו">#REF!</definedName>
+    <definedName name="ליקרים_דזסטיף">#REF!</definedName>
+    <definedName name="פנינים">#REF!</definedName>
+    <definedName name="רום">#REF!</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
   <si>
     <t xml:space="preserve">שם החנות </t>
   </si>
@@ -111,168 +110,6 @@
     <t xml:space="preserve">רום </t>
   </si>
   <si>
-    <t>ג'וני ווקר רד לייבל</t>
-  </si>
-  <si>
-    <t>ג'וני ווקר בלאק לייבל</t>
-  </si>
-  <si>
-    <t>ג'וני ווקר דאבל בלאק</t>
-  </si>
-  <si>
-    <t>ג'וני ווקר גרין לייבל</t>
-  </si>
-  <si>
-    <t>ג'וני ווקר גולד רזרב</t>
-  </si>
-  <si>
-    <t>ג'וני ווקר פלטינום</t>
-  </si>
-  <si>
-    <t>ג'וני ווקר בלו לייבל</t>
-  </si>
-  <si>
-    <t>J&amp;B</t>
-  </si>
-  <si>
-    <t>J&amp;B RESERVE</t>
-  </si>
-  <si>
-    <t>B&amp;W</t>
-  </si>
-  <si>
-    <t>דימפל 15</t>
-  </si>
-  <si>
-    <t>קראון רויאל</t>
-  </si>
-  <si>
-    <t>ווילד טורקי 81</t>
-  </si>
-  <si>
-    <t>ווילד טורקי 101</t>
-  </si>
-  <si>
-    <t>בושמילס</t>
-  </si>
-  <si>
-    <t>בושמילס 10</t>
-  </si>
-  <si>
-    <t>בושמילס 16</t>
-  </si>
-  <si>
-    <t>בושמילס 21</t>
-  </si>
-  <si>
-    <t>גלן קינצ'י</t>
-  </si>
-  <si>
-    <t>דלוויני</t>
-  </si>
-  <si>
-    <t>רויאל לוכנגר</t>
-  </si>
-  <si>
-    <t>גלן גרנט</t>
-  </si>
-  <si>
-    <t>גלן אלגין</t>
-  </si>
-  <si>
-    <t>קליינאליש</t>
-  </si>
-  <si>
-    <t>קראגנאמור</t>
-  </si>
-  <si>
-    <t>קטל וואן</t>
-  </si>
-  <si>
-    <t>קטל וואן טעמים</t>
-  </si>
-  <si>
-    <t>טנקרי סטרלינג</t>
-  </si>
-  <si>
-    <t>סירוק</t>
-  </si>
-  <si>
-    <t>סמירנוף בלו</t>
-  </si>
-  <si>
-    <t>סמירנוף בלאק</t>
-  </si>
-  <si>
-    <t>סמירנוף טעמים</t>
-  </si>
-  <si>
-    <t>פמפרו בלאנקו</t>
-  </si>
-  <si>
-    <t>קפטן מורגן ספייסד</t>
-  </si>
-  <si>
-    <t>קפטן מורגן בלאק</t>
-  </si>
-  <si>
-    <t xml:space="preserve">מאיירס </t>
-  </si>
-  <si>
-    <t>זאקאפה 23</t>
-  </si>
-  <si>
-    <t>זאקאפה XO</t>
-  </si>
-  <si>
-    <t>גורדונס</t>
-  </si>
-  <si>
-    <t>טנקרי 10</t>
-  </si>
-  <si>
-    <t>טנקרי</t>
-  </si>
-  <si>
-    <t>דון חוליו בלאנקו</t>
-  </si>
-  <si>
-    <t>דון חוליו רפוסאדו</t>
-  </si>
-  <si>
-    <t>דון חוליו אניחו</t>
-  </si>
-  <si>
-    <t>אפרול</t>
-  </si>
-  <si>
-    <t>קמפרי</t>
-  </si>
-  <si>
-    <t>שרידאנס</t>
-  </si>
-  <si>
-    <t>זוואק יוניקום</t>
-  </si>
-  <si>
-    <t>אוזו 12</t>
-  </si>
-  <si>
-    <t>ערק פיירוז</t>
-  </si>
-  <si>
-    <t>ערק אל נמרוד</t>
-  </si>
-  <si>
-    <t>ערק אל נמרוד מיושן בחביות</t>
-  </si>
-  <si>
-    <t>צנזאנו ביאנקו</t>
-  </si>
-  <si>
-    <t>צנזאנו רוסו</t>
-  </si>
-  <si>
     <t>ליקרים_דזסטיף</t>
   </si>
   <si>
@@ -288,66 +125,6 @@
     <t>גין</t>
   </si>
   <si>
-    <t>צנזאנו אקסטרה דריי</t>
-  </si>
-  <si>
-    <t>ארצרס שנאפס</t>
-  </si>
-  <si>
-    <t>קברנה סוביניון</t>
-  </si>
-  <si>
-    <t>מרלו</t>
-  </si>
-  <si>
-    <t>שיראז</t>
-  </si>
-  <si>
-    <t>שרדונה</t>
-  </si>
-  <si>
-    <t>סוביניון בלאן</t>
-  </si>
-  <si>
-    <t>רוסאן</t>
-  </si>
-  <si>
-    <t>גוורצטרמינר</t>
-  </si>
-  <si>
-    <t>מרלו_פטיט ורדו</t>
-  </si>
-  <si>
-    <t>_</t>
-  </si>
-  <si>
-    <t>קברנה סוביניון_מורבדרה</t>
-  </si>
-  <si>
-    <t>קברנה סוביניון_מרלו</t>
-  </si>
-  <si>
-    <t>קברנה סוביניון_קברנה פרנק</t>
-  </si>
-  <si>
-    <t>בציר_2007_1_מתוך_7000</t>
-  </si>
-  <si>
-    <t>בציר_2008_1_מתוך_19000</t>
-  </si>
-  <si>
-    <t>בציר_2009_1_מתוך_11000</t>
-  </si>
-  <si>
-    <t>לבן</t>
-  </si>
-  <si>
-    <t>רוזה</t>
-  </si>
-  <si>
-    <t>אדום</t>
-  </si>
-  <si>
     <t>בקבוקי טעימה:</t>
   </si>
   <si>
@@ -357,52 +134,10 @@
     <t>פנינים</t>
   </si>
   <si>
-    <t>ברוט</t>
-  </si>
-  <si>
-    <t>צינזנו_אסטי</t>
-  </si>
-  <si>
-    <t>צינזנו_פרוסקו</t>
-  </si>
-  <si>
-    <t>צינזנו_גראן_דולצה</t>
-  </si>
-  <si>
-    <t>צינזנו_רוז</t>
-  </si>
-  <si>
-    <t>מארז_אפרול_פרסקו</t>
-  </si>
-  <si>
-    <t>מארז_אפרול_562</t>
-  </si>
-  <si>
-    <t>בושמילס דבש</t>
-  </si>
-  <si>
     <t>היו אנשים? המנהל התנהג כמו שצריך? כל הציוד של ייעוץ האלכוהול עמד לרשתוכם? מכירות נמוכות אז מדוע? ועוד ועוד....</t>
   </si>
   <si>
-    <t>מארז קמפרי עם כוס</t>
-  </si>
-  <si>
     <t>אדמה_2_חדשה</t>
-  </si>
-  <si>
-    <t>טללים</t>
-  </si>
-  <si>
-    <t>רעם</t>
-  </si>
-  <si>
-    <t>סופה</t>
-  </si>
-  <si>
-    <t>קשת</t>
-  </si>
-  <si>
-    <t>להבה</t>
   </si>
   <si>
     <t>הר</t>
@@ -415,60 +150,6 @@
   </si>
   <si>
     <t>כמות שנפתחה (אין להטעים בקבוק שהיה פתוח כבר)</t>
-  </si>
-  <si>
-    <t>סמירנוף אדום</t>
-  </si>
-  <si>
-    <t>בייליס שוקולד</t>
-  </si>
-  <si>
-    <t>בייליס קלאסי</t>
-  </si>
-  <si>
-    <t>ויונייה</t>
-  </si>
-  <si>
-    <t>גורדונס מלפפון</t>
-  </si>
-  <si>
-    <t>בולט ברבן</t>
-  </si>
-  <si>
-    <t>קרדו גולד רזרב</t>
-  </si>
-  <si>
-    <t>קרדו 12</t>
-  </si>
-  <si>
-    <t>סינגלטון 12</t>
-  </si>
-  <si>
-    <t>סינגלטון 15</t>
-  </si>
-  <si>
-    <t>סינגלטון 18</t>
-  </si>
-  <si>
-    <t>טליסקר 10</t>
-  </si>
-  <si>
-    <t>טליסקר STORM</t>
-  </si>
-  <si>
-    <t>טליסקר 18</t>
-  </si>
-  <si>
-    <t>טליסקר 25</t>
-  </si>
-  <si>
-    <t>בולט ריי (שיפון)</t>
-  </si>
-  <si>
-    <t>קאול איילה</t>
-  </si>
-  <si>
-    <t>לאגאבולין</t>
   </si>
   <si>
     <t>סה"כ ללא רד לייבל ובלאק לייבל</t>
@@ -509,31 +190,10 @@
     <t>סה"כ בלק לייבל</t>
   </si>
   <si>
-    <t>בלאק בוש</t>
-  </si>
-  <si>
-    <t>טליסקר 30</t>
-  </si>
-  <si>
-    <t>שחר</t>
-  </si>
-  <si>
     <t>הערות והמלצות-</t>
   </si>
   <si>
-    <t>סינגלטון תל פייר</t>
-  </si>
-  <si>
-    <t>בציר_2010_1_מתוך_11001</t>
-  </si>
-  <si>
-    <t>FEVER TREE</t>
-  </si>
-  <si>
     <t>fever_tree</t>
-  </si>
-  <si>
-    <t>פרנג'ליקו</t>
   </si>
 </sst>
 </file>
@@ -1214,7 +874,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1255,12 +915,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1367,111 +1021,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1481,6 +1030,112 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1579,13 +1234,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>94</xdr:row>
+      <xdr:row>122</xdr:row>
       <xdr:rowOff>29633</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>194734</xdr:colOff>
-      <xdr:row>97</xdr:row>
+      <xdr:row>125</xdr:row>
       <xdr:rowOff>67733</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1727,14 +1382,14 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>351367</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>106</xdr:row>
       <xdr:rowOff>143933</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>630767</xdr:colOff>
-      <xdr:row>82</xdr:row>
-      <xdr:rowOff>198967</xdr:rowOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>198966</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1801,13 +1456,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>173567</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>95</xdr:row>
       <xdr:rowOff>21167</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>102</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1949,14 +1604,14 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>359833</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>87</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2023,13 +1678,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>143933</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>8467</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>702733</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>91</xdr:row>
       <xdr:rowOff>173567</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2097,13 +1752,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>160867</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>8467</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>376767</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>83</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2171,13 +1826,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>173567</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>29633</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2245,14 +1900,14 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>160867</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>104</xdr:row>
       <xdr:rowOff>8467</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>97367</xdr:rowOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>97368</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2319,13 +1974,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>91</xdr:row>
       <xdr:rowOff>97367</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>423333</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>94</xdr:row>
       <xdr:rowOff>97367</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2392,15 +2047,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>135467</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>97367</xdr:rowOff>
+      <xdr:colOff>173567</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>63501</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>131233</xdr:rowOff>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>97368</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2430,8 +2085,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="162479567" y="6642100"/>
-          <a:ext cx="1824566" cy="762000"/>
+          <a:off x="10541732366" y="9537701"/>
+          <a:ext cx="1824567" cy="762000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2467,14 +2122,14 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>313267</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>97367</xdr:rowOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>97368</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2540,15 +2195,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>80433</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>59267</xdr:rowOff>
+      <xdr:colOff>156633</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>33866</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>12699</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2578,8 +2233,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="157729767" y="6786033"/>
-          <a:ext cx="1485900" cy="524934"/>
+          <a:off x="10535483966" y="8398933"/>
+          <a:ext cx="1485901" cy="524933"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2613,16 +2268,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>736600</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>97367</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1926166</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>25401</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>833966</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>148167</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2652,8 +2307,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="158889700" y="5731933"/>
-          <a:ext cx="2214033" cy="1032934"/>
+          <a:off x="10537973167" y="7662334"/>
+          <a:ext cx="2214033" cy="1032933"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2688,15 +2343,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>740834</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>173567</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>160867</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>160867</xdr:rowOff>
+      <xdr:colOff>622301</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2726,7 +2381,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="158512933" y="5202767"/>
+          <a:off x="10535881899" y="7082367"/>
           <a:ext cx="1257300" cy="410633"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2910,15 +2565,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>711200</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>1058333</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1468966</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>29633</xdr:rowOff>
+      <xdr:colOff>1816099</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>127001</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2948,8 +2603,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="161353500" y="6544733"/>
-          <a:ext cx="757767" cy="757767"/>
+          <a:off x="10540297267" y="8843434"/>
+          <a:ext cx="757766" cy="757767"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3305,10 +2960,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:N95"/>
+  <dimension ref="A4:N123"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E66" sqref="A59:E66"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:XFD57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
@@ -3329,59 +2984,59 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84"/>
-      <c r="K4" s="84"/>
+      <c r="B4" s="87"/>
+      <c r="C4" s="87"/>
+      <c r="D4" s="87"/>
+      <c r="E4" s="87"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="87"/>
+      <c r="K4" s="87"/>
     </row>
     <row r="5" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A5" s="84"/>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="84"/>
-      <c r="K5" s="84"/>
+      <c r="A5" s="87"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="87"/>
+      <c r="K5" s="87"/>
     </row>
     <row r="6" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A6" s="84"/>
-      <c r="B6" s="84"/>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="84"/>
-      <c r="I6" s="84"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="84"/>
+      <c r="A6" s="87"/>
+      <c r="B6" s="87"/>
+      <c r="C6" s="87"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="87"/>
     </row>
     <row r="8" spans="1:12" ht="14.7" thickBot="1">
-      <c r="C8" s="75"/>
+      <c r="C8" s="73"/>
     </row>
     <row r="9" spans="1:12" ht="14.7" thickBot="1">
       <c r="A9" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="77"/>
-      <c r="C9" s="76"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="74"/>
       <c r="D9" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="74"/>
+      <c r="E9" s="72"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="K9" s="4"/>
@@ -3399,12 +3054,12 @@
       <c r="A11" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="77"/>
-      <c r="C11" s="76"/>
+      <c r="B11" s="75"/>
+      <c r="C11" s="74"/>
       <c r="D11" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="E11" s="74"/>
+        <v>30</v>
+      </c>
+      <c r="E11" s="72"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="K11" s="4"/>
@@ -3422,26 +3077,26 @@
       <c r="A13" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="77"/>
-      <c r="C13" s="76"/>
+      <c r="B13" s="75"/>
+      <c r="C13" s="74"/>
       <c r="D13" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="74"/>
+      <c r="E13" s="72"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="K13" s="4"/>
     </row>
     <row r="15" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A15" s="67" t="s">
+      <c r="A15" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="67"/>
-      <c r="C15" s="82"/>
-      <c r="D15" s="82"/>
-      <c r="E15" s="82"/>
-      <c r="F15" s="68"/>
-      <c r="G15" s="68"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="8"/>
@@ -3449,8 +3104,8 @@
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:12" ht="17.25" hidden="1" customHeight="1">
-      <c r="A16" s="80"/>
-      <c r="B16" s="80"/>
+      <c r="A16" s="78"/>
+      <c r="B16" s="78"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -3463,10 +3118,10 @@
       <c r="L16" s="7"/>
     </row>
     <row r="17" spans="1:12" ht="17.25" customHeight="1">
-      <c r="A17" s="123" t="s">
+      <c r="A17" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="123" t="s">
+      <c r="B17" s="86" t="s">
         <v>22</v>
       </c>
       <c r="C17" s="7"/>
@@ -3481,8 +3136,8 @@
       <c r="L17" s="7"/>
     </row>
     <row r="18" spans="1:12" ht="17.25" customHeight="1">
-      <c r="A18" s="59"/>
-      <c r="B18" s="59"/>
+      <c r="A18" s="57"/>
+      <c r="B18" s="57"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
@@ -3495,8 +3150,8 @@
       <c r="L18" s="7"/>
     </row>
     <row r="19" spans="1:12" ht="17.25" customHeight="1">
-      <c r="A19" s="59"/>
-      <c r="B19" s="59"/>
+      <c r="A19" s="57"/>
+      <c r="B19" s="57"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
@@ -3509,1635 +3164,1479 @@
       <c r="L19" s="7"/>
     </row>
     <row r="20" spans="1:12" ht="17.25" customHeight="1">
-      <c r="A20" s="59"/>
-      <c r="B20" s="59"/>
-      <c r="C20" s="121"/>
-      <c r="D20" s="121"/>
-      <c r="E20" s="122"/>
-      <c r="F20" s="122"/>
-      <c r="G20" s="122"/>
-      <c r="H20" s="122"/>
-      <c r="I20" s="122"/>
+      <c r="A20" s="57"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="84"/>
+      <c r="D20" s="84"/>
+      <c r="E20" s="85"/>
+      <c r="F20" s="85"/>
+      <c r="G20" s="85"/>
+      <c r="H20" s="85"/>
+      <c r="I20" s="85"/>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
       <c r="L20" s="7"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="59"/>
-      <c r="B21" s="59"/>
-      <c r="C21" s="83"/>
-      <c r="D21" s="83"/>
-      <c r="E21" s="83"/>
-      <c r="F21" s="83"/>
-      <c r="G21" s="83"/>
-      <c r="H21" s="83"/>
-      <c r="I21" s="83"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="81"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
+      <c r="F21" s="81"/>
+      <c r="G21" s="81"/>
+      <c r="H21" s="81"/>
+      <c r="I21" s="81"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="59"/>
-      <c r="B22" s="59"/>
-      <c r="C22" s="83"/>
-      <c r="D22" s="83"/>
-      <c r="E22" s="83"/>
-      <c r="F22" s="83"/>
-      <c r="G22" s="83"/>
-      <c r="H22" s="83"/>
-      <c r="I22" s="83"/>
+      <c r="A22" s="57"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="81"/>
+      <c r="D22" s="81"/>
+      <c r="E22" s="81"/>
+      <c r="F22" s="81"/>
+      <c r="G22" s="81"/>
+      <c r="H22" s="81"/>
+      <c r="I22" s="81"/>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="59"/>
-      <c r="B23" s="59"/>
-      <c r="C23" s="83"/>
-      <c r="D23" s="83"/>
-      <c r="E23" s="83"/>
-      <c r="F23" s="83"/>
-      <c r="G23" s="83"/>
-      <c r="H23" s="83"/>
-      <c r="I23" s="83"/>
+      <c r="A23" s="57"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="81"/>
+      <c r="D23" s="81"/>
+      <c r="E23" s="81"/>
+      <c r="F23" s="81"/>
+      <c r="G23" s="81"/>
+      <c r="H23" s="81"/>
+      <c r="I23" s="81"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
       <c r="L23" s="9"/>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="59"/>
-      <c r="B24" s="59"/>
-      <c r="C24" s="83"/>
-      <c r="D24" s="83"/>
-      <c r="E24" s="83"/>
-      <c r="F24" s="83"/>
-      <c r="G24" s="83"/>
-      <c r="H24" s="83"/>
-      <c r="I24" s="83"/>
+      <c r="A24" s="57"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="81"/>
+      <c r="G24" s="81"/>
+      <c r="H24" s="81"/>
+      <c r="I24" s="81"/>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
       <c r="L24" s="9"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="59"/>
-      <c r="B25" s="59"/>
-      <c r="C25" s="83"/>
-      <c r="D25" s="83"/>
-      <c r="E25" s="83"/>
-      <c r="F25" s="83"/>
-      <c r="G25" s="83"/>
-      <c r="H25" s="83"/>
-      <c r="I25" s="83"/>
+      <c r="A25" s="57"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="81"/>
+      <c r="D25" s="81"/>
+      <c r="E25" s="81"/>
+      <c r="F25" s="81"/>
+      <c r="G25" s="81"/>
+      <c r="H25" s="81"/>
+      <c r="I25" s="81"/>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
       <c r="L25" s="9"/>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="59"/>
-      <c r="B26" s="59"/>
-      <c r="C26" s="119"/>
-      <c r="D26" s="83"/>
-      <c r="E26" s="83"/>
-      <c r="F26" s="119"/>
-      <c r="G26" s="83"/>
-      <c r="H26" s="83"/>
-      <c r="I26" s="83"/>
+      <c r="A26" s="57"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="82"/>
+      <c r="D26" s="81"/>
+      <c r="E26" s="81"/>
+      <c r="F26" s="82"/>
+      <c r="G26" s="81"/>
+      <c r="H26" s="81"/>
+      <c r="I26" s="81"/>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="59"/>
-      <c r="B27" s="59"/>
-      <c r="C27" s="119"/>
-      <c r="D27" s="83"/>
-      <c r="E27" s="83"/>
-      <c r="F27" s="119"/>
-      <c r="G27" s="83"/>
-      <c r="H27" s="83"/>
-      <c r="I27" s="83"/>
+      <c r="A27" s="57"/>
+      <c r="B27" s="57"/>
+      <c r="C27" s="82"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
+      <c r="F27" s="82"/>
+      <c r="G27" s="81"/>
+      <c r="H27" s="81"/>
+      <c r="I27" s="81"/>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="59"/>
-      <c r="B28" s="59"/>
-      <c r="C28" s="83"/>
-      <c r="D28" s="83"/>
-      <c r="E28" s="83"/>
-      <c r="F28" s="119"/>
-      <c r="G28" s="83"/>
-      <c r="H28" s="83"/>
-      <c r="I28" s="83"/>
+      <c r="A28" s="57"/>
+      <c r="B28" s="57"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="81"/>
+      <c r="E28" s="81"/>
+      <c r="F28" s="82"/>
+      <c r="G28" s="81"/>
+      <c r="H28" s="81"/>
+      <c r="I28" s="81"/>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="59"/>
-      <c r="B29" s="59"/>
-      <c r="C29" s="83"/>
-      <c r="D29" s="83"/>
-      <c r="E29" s="83"/>
-      <c r="F29" s="119"/>
-      <c r="G29" s="119"/>
-      <c r="H29" s="83"/>
-      <c r="I29" s="83"/>
+      <c r="A29" s="57"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="82"/>
+      <c r="D29" s="81"/>
+      <c r="E29" s="81"/>
+      <c r="F29" s="82"/>
+      <c r="G29" s="81"/>
+      <c r="H29" s="81"/>
+      <c r="I29" s="81"/>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
       <c r="L29" s="9"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="59"/>
-      <c r="B30" s="59"/>
-      <c r="C30" s="83"/>
-      <c r="D30" s="83"/>
-      <c r="E30" s="83"/>
-      <c r="F30" s="83"/>
-      <c r="G30" s="119"/>
-      <c r="H30" s="83"/>
-      <c r="I30" s="83"/>
+      <c r="A30" s="57"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="82"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="81"/>
+      <c r="F30" s="82"/>
+      <c r="G30" s="81"/>
+      <c r="H30" s="81"/>
+      <c r="I30" s="81"/>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="59"/>
-      <c r="B31" s="59"/>
-      <c r="C31" s="83"/>
-      <c r="D31" s="83"/>
-      <c r="E31" s="83"/>
-      <c r="F31" s="83"/>
-      <c r="G31" s="119"/>
-      <c r="H31" s="83"/>
-      <c r="I31" s="83"/>
+      <c r="A31" s="57"/>
+      <c r="B31" s="57"/>
+      <c r="C31" s="82"/>
+      <c r="D31" s="81"/>
+      <c r="E31" s="81"/>
+      <c r="F31" s="82"/>
+      <c r="G31" s="81"/>
+      <c r="H31" s="81"/>
+      <c r="I31" s="81"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
       <c r="L31" s="9"/>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="59"/>
-      <c r="B32" s="59"/>
-      <c r="C32" s="83"/>
-      <c r="D32" s="83"/>
-      <c r="E32" s="83"/>
-      <c r="F32" s="83"/>
-      <c r="G32" s="119"/>
-      <c r="H32" s="83"/>
-      <c r="I32" s="83"/>
+      <c r="A32" s="57"/>
+      <c r="B32" s="57"/>
+      <c r="C32" s="82"/>
+      <c r="D32" s="81"/>
+      <c r="E32" s="81"/>
+      <c r="F32" s="82"/>
+      <c r="G32" s="81"/>
+      <c r="H32" s="81"/>
+      <c r="I32" s="81"/>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
       <c r="L32" s="9"/>
     </row>
-    <row r="33" spans="1:14">
-      <c r="A33" s="59"/>
-      <c r="B33" s="59"/>
-      <c r="C33" s="83"/>
-      <c r="D33" s="83"/>
-      <c r="E33" s="119"/>
-      <c r="F33" s="119"/>
-      <c r="G33" s="119"/>
-      <c r="H33" s="83"/>
-      <c r="I33" s="83"/>
+    <row r="33" spans="1:12">
+      <c r="A33" s="57"/>
+      <c r="B33" s="57"/>
+      <c r="C33" s="82"/>
+      <c r="D33" s="81"/>
+      <c r="E33" s="81"/>
+      <c r="F33" s="82"/>
+      <c r="G33" s="81"/>
+      <c r="H33" s="81"/>
+      <c r="I33" s="81"/>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
       <c r="L33" s="9"/>
     </row>
-    <row r="34" spans="1:14">
-      <c r="A34" s="119"/>
-      <c r="B34" s="83"/>
-      <c r="C34" s="83"/>
-      <c r="D34" s="83"/>
-      <c r="E34" s="120"/>
-      <c r="F34" s="119"/>
-      <c r="G34" s="119"/>
-      <c r="H34" s="83"/>
-      <c r="I34" s="83"/>
+    <row r="34" spans="1:12">
+      <c r="A34" s="57"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="82"/>
+      <c r="D34" s="81"/>
+      <c r="E34" s="81"/>
+      <c r="F34" s="82"/>
+      <c r="G34" s="81"/>
+      <c r="H34" s="81"/>
+      <c r="I34" s="81"/>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
       <c r="L34" s="9"/>
     </row>
-    <row r="35" spans="1:14">
-      <c r="A35" s="119"/>
-      <c r="B35" s="83"/>
-      <c r="C35" s="83"/>
-      <c r="D35" s="83"/>
-      <c r="E35" s="119"/>
-      <c r="F35" s="119"/>
-      <c r="G35" s="119"/>
-      <c r="H35" s="83"/>
-      <c r="I35" s="83"/>
+    <row r="35" spans="1:12">
+      <c r="A35" s="57"/>
+      <c r="B35" s="57"/>
+      <c r="C35" s="82"/>
+      <c r="D35" s="81"/>
+      <c r="E35" s="81"/>
+      <c r="F35" s="82"/>
+      <c r="G35" s="81"/>
+      <c r="H35" s="81"/>
+      <c r="I35" s="81"/>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
       <c r="L35" s="9"/>
     </row>
-    <row r="36" spans="1:14">
-      <c r="A36" s="119"/>
-      <c r="B36" s="83"/>
-      <c r="C36" s="83"/>
-      <c r="D36" s="119"/>
-      <c r="E36" s="119"/>
-      <c r="F36" s="119"/>
-      <c r="G36" s="83"/>
-      <c r="H36" s="83"/>
-      <c r="I36" s="83"/>
+    <row r="36" spans="1:12">
+      <c r="A36" s="57"/>
+      <c r="B36" s="57"/>
+      <c r="C36" s="82"/>
+      <c r="D36" s="81"/>
+      <c r="E36" s="81"/>
+      <c r="F36" s="82"/>
+      <c r="G36" s="81"/>
+      <c r="H36" s="81"/>
+      <c r="I36" s="81"/>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
       <c r="L36" s="9"/>
-      <c r="M36" s="75"/>
-      <c r="N36" s="75"/>
-    </row>
-    <row r="37" spans="1:14">
-      <c r="A37" s="119"/>
-      <c r="B37" s="83"/>
-      <c r="C37" s="83"/>
-      <c r="D37" s="119"/>
-      <c r="E37" s="119"/>
-      <c r="F37" s="119"/>
-      <c r="G37" s="83"/>
-      <c r="H37" s="83"/>
-      <c r="I37" s="83"/>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="57"/>
+      <c r="B37" s="57"/>
+      <c r="C37" s="82"/>
+      <c r="D37" s="81"/>
+      <c r="E37" s="81"/>
+      <c r="F37" s="82"/>
+      <c r="G37" s="81"/>
+      <c r="H37" s="81"/>
+      <c r="I37" s="81"/>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
       <c r="L37" s="9"/>
-      <c r="M37" s="75"/>
-      <c r="N37" s="75"/>
-    </row>
-    <row r="38" spans="1:14">
-      <c r="A38" s="119"/>
-      <c r="B38" s="83"/>
-      <c r="C38" s="83"/>
-      <c r="D38" s="119"/>
-      <c r="E38" s="119"/>
-      <c r="F38" s="119"/>
-      <c r="G38" s="83"/>
-      <c r="H38" s="83"/>
-      <c r="I38" s="83"/>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="57"/>
+      <c r="B38" s="57"/>
+      <c r="C38" s="82"/>
+      <c r="D38" s="81"/>
+      <c r="E38" s="81"/>
+      <c r="F38" s="82"/>
+      <c r="G38" s="81"/>
+      <c r="H38" s="81"/>
+      <c r="I38" s="81"/>
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
       <c r="L38" s="9"/>
-      <c r="M38" s="75"/>
-      <c r="N38" s="75"/>
-    </row>
-    <row r="39" spans="1:14">
-      <c r="A39" s="119"/>
-      <c r="B39" s="83"/>
-      <c r="C39" s="83"/>
-      <c r="D39" s="83"/>
-      <c r="E39" s="83"/>
-      <c r="F39" s="83"/>
-      <c r="G39" s="83"/>
-      <c r="H39" s="83"/>
-      <c r="I39" s="83"/>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="57"/>
+      <c r="B39" s="57"/>
+      <c r="C39" s="82"/>
+      <c r="D39" s="81"/>
+      <c r="E39" s="81"/>
+      <c r="F39" s="82"/>
+      <c r="G39" s="81"/>
+      <c r="H39" s="81"/>
+      <c r="I39" s="81"/>
       <c r="J39" s="9"/>
       <c r="K39" s="9"/>
       <c r="L39" s="9"/>
-      <c r="M39" s="75"/>
-      <c r="N39" s="75"/>
-    </row>
-    <row r="40" spans="1:14">
-      <c r="A40" s="119"/>
-      <c r="B40" s="83"/>
-      <c r="C40" s="119"/>
-      <c r="D40" s="119"/>
-      <c r="E40" s="119"/>
-      <c r="F40" s="119"/>
-      <c r="G40" s="119"/>
-      <c r="H40" s="119"/>
-      <c r="I40" s="119"/>
-      <c r="J40" s="75"/>
-      <c r="K40" s="75"/>
-      <c r="L40" s="75"/>
-      <c r="M40" s="75"/>
-      <c r="N40" s="75"/>
-    </row>
-    <row r="41" spans="1:14" ht="14.7" thickBot="1">
-      <c r="B41" s="63"/>
-      <c r="C41" s="75"/>
-      <c r="D41" s="75"/>
-      <c r="E41" s="75"/>
-      <c r="F41" s="75"/>
-      <c r="G41" s="75"/>
-      <c r="H41" s="75"/>
-      <c r="I41" s="75"/>
-      <c r="J41" s="75"/>
-      <c r="K41" s="75"/>
-      <c r="L41" s="75"/>
-      <c r="M41" s="75"/>
-      <c r="N41" s="75"/>
-    </row>
-    <row r="42" spans="1:14" ht="25">
-      <c r="A42" s="116" t="s">
-        <v>103</v>
-      </c>
-      <c r="B42" s="117"/>
-      <c r="C42" s="117"/>
-      <c r="D42" s="118"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="107" t="s">
-        <v>103</v>
-      </c>
-      <c r="G42" s="108"/>
-      <c r="H42" s="108"/>
-      <c r="I42" s="109"/>
-      <c r="K42" s="5"/>
-    </row>
-    <row r="43" spans="1:14" ht="20.350000000000001" thickBot="1">
-      <c r="A43" s="113" t="s">
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="57"/>
+      <c r="B40" s="57"/>
+      <c r="C40" s="82"/>
+      <c r="D40" s="81"/>
+      <c r="E40" s="81"/>
+      <c r="F40" s="82"/>
+      <c r="G40" s="81"/>
+      <c r="H40" s="81"/>
+      <c r="I40" s="81"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="57"/>
+      <c r="B41" s="57"/>
+      <c r="C41" s="82"/>
+      <c r="D41" s="81"/>
+      <c r="E41" s="81"/>
+      <c r="F41" s="82"/>
+      <c r="G41" s="81"/>
+      <c r="H41" s="81"/>
+      <c r="I41" s="81"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="57"/>
+      <c r="B42" s="57"/>
+      <c r="C42" s="82"/>
+      <c r="D42" s="81"/>
+      <c r="E42" s="81"/>
+      <c r="F42" s="82"/>
+      <c r="G42" s="81"/>
+      <c r="H42" s="81"/>
+      <c r="I42" s="81"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="57"/>
+      <c r="B43" s="57"/>
+      <c r="C43" s="82"/>
+      <c r="D43" s="81"/>
+      <c r="E43" s="81"/>
+      <c r="F43" s="82"/>
+      <c r="G43" s="81"/>
+      <c r="H43" s="81"/>
+      <c r="I43" s="81"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="9"/>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" s="57"/>
+      <c r="B44" s="57"/>
+      <c r="C44" s="82"/>
+      <c r="D44" s="81"/>
+      <c r="E44" s="81"/>
+      <c r="F44" s="82"/>
+      <c r="G44" s="81"/>
+      <c r="H44" s="81"/>
+      <c r="I44" s="81"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="9"/>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" s="57"/>
+      <c r="B45" s="57"/>
+      <c r="C45" s="82"/>
+      <c r="D45" s="81"/>
+      <c r="E45" s="81"/>
+      <c r="F45" s="82"/>
+      <c r="G45" s="81"/>
+      <c r="H45" s="81"/>
+      <c r="I45" s="81"/>
+      <c r="J45" s="9"/>
+      <c r="K45" s="9"/>
+      <c r="L45" s="9"/>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="57"/>
+      <c r="B46" s="57"/>
+      <c r="C46" s="82"/>
+      <c r="D46" s="81"/>
+      <c r="E46" s="81"/>
+      <c r="F46" s="82"/>
+      <c r="G46" s="81"/>
+      <c r="H46" s="81"/>
+      <c r="I46" s="81"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="9"/>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="57"/>
+      <c r="B47" s="57"/>
+      <c r="C47" s="82"/>
+      <c r="D47" s="81"/>
+      <c r="E47" s="81"/>
+      <c r="F47" s="82"/>
+      <c r="G47" s="81"/>
+      <c r="H47" s="81"/>
+      <c r="I47" s="81"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="9"/>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" s="57"/>
+      <c r="B48" s="57"/>
+      <c r="C48" s="82"/>
+      <c r="D48" s="81"/>
+      <c r="E48" s="81"/>
+      <c r="F48" s="82"/>
+      <c r="G48" s="81"/>
+      <c r="H48" s="81"/>
+      <c r="I48" s="81"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49" s="57"/>
+      <c r="B49" s="57"/>
+      <c r="C49" s="82"/>
+      <c r="D49" s="81"/>
+      <c r="E49" s="81"/>
+      <c r="F49" s="82"/>
+      <c r="G49" s="81"/>
+      <c r="H49" s="81"/>
+      <c r="I49" s="81"/>
+      <c r="J49" s="9"/>
+      <c r="K49" s="9"/>
+      <c r="L49" s="9"/>
+    </row>
+    <row r="50" spans="1:14">
+      <c r="A50" s="57"/>
+      <c r="B50" s="57"/>
+      <c r="C50" s="82"/>
+      <c r="D50" s="81"/>
+      <c r="E50" s="81"/>
+      <c r="F50" s="82"/>
+      <c r="G50" s="81"/>
+      <c r="H50" s="81"/>
+      <c r="I50" s="81"/>
+      <c r="J50" s="9"/>
+      <c r="K50" s="9"/>
+      <c r="L50" s="9"/>
+    </row>
+    <row r="51" spans="1:14" ht="15.7" customHeight="1">
+      <c r="A51" s="57"/>
+      <c r="B51" s="57"/>
+      <c r="C51" s="82"/>
+      <c r="D51" s="81"/>
+      <c r="E51" s="81"/>
+      <c r="F51" s="82"/>
+      <c r="G51" s="81"/>
+      <c r="H51" s="81"/>
+      <c r="I51" s="81"/>
+      <c r="J51" s="9"/>
+      <c r="K51" s="9"/>
+      <c r="L51" s="9"/>
+    </row>
+    <row r="52" spans="1:14">
+      <c r="A52" s="57"/>
+      <c r="B52" s="57"/>
+      <c r="C52" s="81"/>
+      <c r="D52" s="81"/>
+      <c r="E52" s="81"/>
+      <c r="F52" s="82"/>
+      <c r="G52" s="81"/>
+      <c r="H52" s="81"/>
+      <c r="I52" s="81"/>
+      <c r="J52" s="9"/>
+      <c r="K52" s="9"/>
+      <c r="L52" s="9"/>
+    </row>
+    <row r="53" spans="1:14">
+      <c r="A53" s="57"/>
+      <c r="B53" s="57"/>
+      <c r="C53" s="81"/>
+      <c r="D53" s="81"/>
+      <c r="E53" s="81"/>
+      <c r="F53" s="82"/>
+      <c r="G53" s="82"/>
+      <c r="H53" s="81"/>
+      <c r="I53" s="81"/>
+      <c r="J53" s="9"/>
+      <c r="K53" s="9"/>
+      <c r="L53" s="9"/>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54" s="57"/>
+      <c r="B54" s="57"/>
+      <c r="C54" s="81"/>
+      <c r="D54" s="81"/>
+      <c r="E54" s="81"/>
+      <c r="F54" s="81"/>
+      <c r="G54" s="82"/>
+      <c r="H54" s="81"/>
+      <c r="I54" s="81"/>
+      <c r="J54" s="9"/>
+      <c r="K54" s="9"/>
+      <c r="L54" s="9"/>
+    </row>
+    <row r="55" spans="1:14">
+      <c r="A55" s="57"/>
+      <c r="B55" s="57"/>
+      <c r="C55" s="81"/>
+      <c r="D55" s="81"/>
+      <c r="E55" s="81"/>
+      <c r="F55" s="81"/>
+      <c r="G55" s="82"/>
+      <c r="H55" s="81"/>
+      <c r="I55" s="81"/>
+      <c r="J55" s="9"/>
+      <c r="K55" s="9"/>
+      <c r="L55" s="9"/>
+    </row>
+    <row r="56" spans="1:14">
+      <c r="A56" s="57"/>
+      <c r="B56" s="57"/>
+      <c r="C56" s="81"/>
+      <c r="D56" s="81"/>
+      <c r="E56" s="81"/>
+      <c r="F56" s="81"/>
+      <c r="G56" s="82"/>
+      <c r="H56" s="81"/>
+      <c r="I56" s="81"/>
+      <c r="J56" s="9"/>
+      <c r="K56" s="9"/>
+      <c r="L56" s="9"/>
+    </row>
+    <row r="57" spans="1:14">
+      <c r="A57" s="57"/>
+      <c r="B57" s="57"/>
+      <c r="C57" s="81"/>
+      <c r="D57" s="81"/>
+      <c r="E57" s="82"/>
+      <c r="F57" s="82"/>
+      <c r="G57" s="82"/>
+      <c r="H57" s="81"/>
+      <c r="I57" s="81"/>
+      <c r="J57" s="9"/>
+      <c r="K57" s="9"/>
+      <c r="L57" s="9"/>
+    </row>
+    <row r="58" spans="1:14">
+      <c r="A58" s="82"/>
+      <c r="B58" s="81"/>
+      <c r="C58" s="81"/>
+      <c r="D58" s="81"/>
+      <c r="E58" s="83"/>
+      <c r="F58" s="82"/>
+      <c r="G58" s="82"/>
+      <c r="H58" s="81"/>
+      <c r="I58" s="81"/>
+      <c r="J58" s="9"/>
+      <c r="K58" s="9"/>
+      <c r="L58" s="9"/>
+    </row>
+    <row r="59" spans="1:14">
+      <c r="A59" s="82"/>
+      <c r="B59" s="81"/>
+      <c r="C59" s="81"/>
+      <c r="D59" s="81"/>
+      <c r="E59" s="82"/>
+      <c r="F59" s="82"/>
+      <c r="G59" s="82"/>
+      <c r="H59" s="81"/>
+      <c r="I59" s="81"/>
+      <c r="J59" s="9"/>
+      <c r="K59" s="9"/>
+      <c r="L59" s="9"/>
+    </row>
+    <row r="60" spans="1:14">
+      <c r="A60" s="82"/>
+      <c r="B60" s="81"/>
+      <c r="C60" s="82"/>
+      <c r="D60" s="82"/>
+      <c r="E60" s="82"/>
+      <c r="F60" s="82"/>
+      <c r="G60" s="82"/>
+      <c r="H60" s="82"/>
+      <c r="I60" s="82"/>
+      <c r="J60" s="73"/>
+      <c r="K60" s="73"/>
+      <c r="L60" s="73"/>
+      <c r="M60" s="73"/>
+      <c r="N60" s="73"/>
+    </row>
+    <row r="61" spans="1:14" ht="14.7" thickBot="1">
+      <c r="B61" s="61"/>
+      <c r="C61" s="73"/>
+      <c r="D61" s="73"/>
+      <c r="E61" s="73"/>
+      <c r="F61" s="73"/>
+      <c r="G61" s="73"/>
+      <c r="H61" s="73"/>
+      <c r="I61" s="73"/>
+      <c r="J61" s="73"/>
+      <c r="K61" s="73"/>
+      <c r="L61" s="73"/>
+      <c r="M61" s="73"/>
+      <c r="N61" s="73"/>
+    </row>
+    <row r="62" spans="1:14" ht="25">
+      <c r="A62" s="119" t="s">
+        <v>29</v>
+      </c>
+      <c r="B62" s="120"/>
+      <c r="C62" s="120"/>
+      <c r="D62" s="121"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="110" t="s">
+        <v>29</v>
+      </c>
+      <c r="G62" s="111"/>
+      <c r="H62" s="111"/>
+      <c r="I62" s="112"/>
+      <c r="K62" s="5"/>
+    </row>
+    <row r="63" spans="1:14" ht="20.350000000000001" thickBot="1">
+      <c r="A63" s="116" t="s">
         <v>9</v>
       </c>
-      <c r="B43" s="114"/>
-      <c r="C43" s="114"/>
-      <c r="D43" s="115"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="110" t="s">
+      <c r="B63" s="117"/>
+      <c r="C63" s="117"/>
+      <c r="D63" s="118"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="113" t="s">
         <v>13</v>
       </c>
-      <c r="G43" s="111"/>
-      <c r="H43" s="111"/>
-      <c r="I43" s="112"/>
-    </row>
-    <row r="44" spans="1:14" s="1" customFormat="1" ht="49.5" customHeight="1" thickBot="1">
-      <c r="A44" s="11" t="s">
+      <c r="G63" s="114"/>
+      <c r="H63" s="114"/>
+      <c r="I63" s="115"/>
+    </row>
+    <row r="64" spans="1:14" s="1" customFormat="1" ht="49.5" customHeight="1" thickBot="1">
+      <c r="A64" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="B64" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C44" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="D44" s="14" t="s">
+      <c r="C64" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D64" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="16" t="s">
+      <c r="E64" s="15"/>
+      <c r="F64" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="G44" s="17" t="s">
+      <c r="G64" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H44" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="I44" s="19" t="s">
+      <c r="H64" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="I64" s="19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:14">
-      <c r="A45" s="20"/>
-      <c r="B45" s="21"/>
-      <c r="C45" s="22"/>
-      <c r="D45" s="23"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="27"/>
-    </row>
-    <row r="46" spans="1:14">
-      <c r="A46" s="28"/>
-      <c r="B46" s="21"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="25"/>
-      <c r="H46" s="32"/>
-      <c r="I46" s="33"/>
-    </row>
-    <row r="47" spans="1:14">
-      <c r="A47" s="28"/>
-      <c r="B47" s="21"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="25"/>
-      <c r="H47" s="32"/>
-      <c r="I47" s="33"/>
-    </row>
-    <row r="48" spans="1:14" ht="14.7" thickBot="1">
-      <c r="A48" s="34"/>
-      <c r="B48" s="35"/>
-      <c r="C48" s="36"/>
-      <c r="D48" s="37"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="38"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="40"/>
-      <c r="I48" s="41"/>
-    </row>
-    <row r="49" spans="1:13" ht="20">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-    </row>
-    <row r="50" spans="1:13" ht="20.350000000000001" thickBot="1">
-      <c r="A50" s="42" t="s">
+    <row r="65" spans="1:11" s="1" customFormat="1">
+      <c r="A65" s="20"/>
+      <c r="B65" s="21"/>
+      <c r="C65" s="20"/>
+      <c r="D65" s="21"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="22"/>
+      <c r="G65" s="23"/>
+      <c r="H65" s="24"/>
+      <c r="I65" s="25"/>
+    </row>
+    <row r="66" spans="1:11" s="1" customFormat="1">
+      <c r="A66" s="20"/>
+      <c r="B66" s="21"/>
+      <c r="C66" s="20"/>
+      <c r="D66" s="21"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="22"/>
+      <c r="G66" s="23"/>
+      <c r="H66" s="24"/>
+      <c r="I66" s="25"/>
+    </row>
+    <row r="67" spans="1:11" s="1" customFormat="1">
+      <c r="A67" s="20"/>
+      <c r="B67" s="21"/>
+      <c r="C67" s="20"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="22"/>
+      <c r="G67" s="23"/>
+      <c r="H67" s="24"/>
+      <c r="I67" s="25"/>
+    </row>
+    <row r="68" spans="1:11" s="1" customFormat="1">
+      <c r="A68" s="20"/>
+      <c r="B68" s="21"/>
+      <c r="C68" s="20"/>
+      <c r="D68" s="21"/>
+      <c r="E68" s="15"/>
+      <c r="F68" s="22"/>
+      <c r="G68" s="23"/>
+      <c r="H68" s="24"/>
+      <c r="I68" s="25"/>
+    </row>
+    <row r="69" spans="1:11" s="1" customFormat="1">
+      <c r="A69" s="20"/>
+      <c r="B69" s="21"/>
+      <c r="C69" s="20"/>
+      <c r="D69" s="21"/>
+      <c r="E69" s="15"/>
+      <c r="F69" s="22"/>
+      <c r="G69" s="23"/>
+      <c r="H69" s="24"/>
+      <c r="I69" s="25"/>
+    </row>
+    <row r="70" spans="1:11" s="1" customFormat="1">
+      <c r="A70" s="26"/>
+      <c r="B70" s="21"/>
+      <c r="C70" s="26"/>
+      <c r="D70" s="21"/>
+      <c r="E70" s="15"/>
+      <c r="F70" s="29"/>
+      <c r="G70" s="122"/>
+      <c r="H70" s="30"/>
+      <c r="I70" s="31"/>
+    </row>
+    <row r="71" spans="1:11" s="1" customFormat="1">
+      <c r="A71" s="20"/>
+      <c r="B71" s="21"/>
+      <c r="C71" s="20"/>
+      <c r="D71" s="21"/>
+      <c r="E71" s="15"/>
+      <c r="F71" s="22"/>
+      <c r="G71" s="23"/>
+      <c r="H71" s="22"/>
+      <c r="I71" s="23"/>
+    </row>
+    <row r="72" spans="1:11" s="1" customFormat="1">
+      <c r="A72" s="26"/>
+      <c r="B72" s="21"/>
+      <c r="C72" s="26"/>
+      <c r="D72" s="21"/>
+      <c r="E72" s="15"/>
+      <c r="F72" s="29"/>
+      <c r="G72" s="122"/>
+      <c r="H72" s="29"/>
+      <c r="I72" s="122"/>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73" s="20"/>
+      <c r="B73" s="21"/>
+      <c r="C73" s="20"/>
+      <c r="D73" s="21"/>
+      <c r="E73" s="8"/>
+      <c r="F73" s="22"/>
+      <c r="G73" s="23"/>
+      <c r="H73" s="22"/>
+      <c r="I73" s="23"/>
+    </row>
+    <row r="74" spans="1:11">
+      <c r="A74" s="26"/>
+      <c r="B74" s="21"/>
+      <c r="C74" s="27"/>
+      <c r="D74" s="28"/>
+      <c r="E74" s="8"/>
+      <c r="F74" s="29"/>
+      <c r="G74" s="122"/>
+      <c r="H74" s="29"/>
+      <c r="I74" s="122"/>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="A75" s="26"/>
+      <c r="B75" s="21"/>
+      <c r="C75" s="27"/>
+      <c r="D75" s="28"/>
+      <c r="E75" s="8"/>
+      <c r="F75" s="29"/>
+      <c r="G75" s="23"/>
+      <c r="H75" s="30"/>
+      <c r="I75" s="31"/>
+    </row>
+    <row r="76" spans="1:11" ht="14.7" thickBot="1">
+      <c r="A76" s="32"/>
+      <c r="B76" s="33"/>
+      <c r="C76" s="34"/>
+      <c r="D76" s="35"/>
+      <c r="E76" s="8"/>
+      <c r="F76" s="36"/>
+      <c r="G76" s="37"/>
+      <c r="H76" s="38"/>
+      <c r="I76" s="39"/>
+    </row>
+    <row r="77" spans="1:11" ht="20">
+      <c r="A77" s="2"/>
+      <c r="B77" s="2"/>
+    </row>
+    <row r="78" spans="1:11" ht="20.350000000000001" thickBot="1">
+      <c r="A78" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B50" s="42"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="8"/>
-      <c r="J50" s="8"/>
-      <c r="K50" s="8"/>
-    </row>
-    <row r="51" spans="1:13" ht="17.7" thickBot="1">
-      <c r="A51" s="104"/>
-      <c r="B51" s="105"/>
-      <c r="C51" s="105"/>
-      <c r="D51" s="105"/>
-      <c r="E51" s="105"/>
-      <c r="F51" s="105"/>
-      <c r="G51" s="105"/>
-      <c r="H51" s="105"/>
-      <c r="I51" s="105"/>
-      <c r="J51" s="105"/>
-      <c r="K51" s="106"/>
-    </row>
-    <row r="53" spans="1:13" ht="27.7">
-      <c r="A53" s="96" t="s">
+      <c r="B78" s="40"/>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
+      <c r="H78" s="9"/>
+      <c r="I78" s="8"/>
+      <c r="J78" s="8"/>
+      <c r="K78" s="8"/>
+    </row>
+    <row r="79" spans="1:11" ht="17.7" thickBot="1">
+      <c r="A79" s="107"/>
+      <c r="B79" s="108"/>
+      <c r="C79" s="108"/>
+      <c r="D79" s="108"/>
+      <c r="E79" s="108"/>
+      <c r="F79" s="108"/>
+      <c r="G79" s="108"/>
+      <c r="H79" s="108"/>
+      <c r="I79" s="108"/>
+      <c r="J79" s="108"/>
+      <c r="K79" s="109"/>
+    </row>
+    <row r="81" spans="1:13" ht="27.7">
+      <c r="A81" s="99" t="s">
         <v>16</v>
       </c>
-      <c r="B53" s="96"/>
-      <c r="C53" s="96"/>
-      <c r="D53" s="96"/>
-      <c r="E53" s="96"/>
-      <c r="F53" s="96"/>
-      <c r="G53" s="96"/>
-      <c r="H53" s="96"/>
-      <c r="I53" s="96"/>
-      <c r="J53" s="96"/>
-      <c r="K53" s="96"/>
-    </row>
-    <row r="55" spans="1:13" ht="20">
-      <c r="A55" s="43" t="s">
+      <c r="B81" s="99"/>
+      <c r="C81" s="99"/>
+      <c r="D81" s="99"/>
+      <c r="E81" s="99"/>
+      <c r="F81" s="99"/>
+      <c r="G81" s="99"/>
+      <c r="H81" s="99"/>
+      <c r="I81" s="99"/>
+      <c r="J81" s="99"/>
+      <c r="K81" s="99"/>
+    </row>
+    <row r="83" spans="1:13" ht="20">
+      <c r="A83" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="B55" s="43"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
-      <c r="F55" s="8"/>
-      <c r="G55" s="44" t="s">
+      <c r="B83" s="41"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8"/>
+      <c r="E83" s="8"/>
+      <c r="F83" s="8"/>
+      <c r="G83" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="H55" s="8"/>
-      <c r="I55" s="8"/>
-      <c r="J55" s="8"/>
-    </row>
-    <row r="56" spans="1:13" ht="14.7" thickBot="1">
-      <c r="A56" s="8"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="8"/>
-      <c r="G56" s="8"/>
-      <c r="H56" s="8"/>
-      <c r="I56" s="8"/>
-      <c r="J56" s="8"/>
-    </row>
-    <row r="57" spans="1:13" s="3" customFormat="1" ht="16" thickBot="1">
-      <c r="A57" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="B57" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="C57" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="D57" s="47" t="s">
-        <v>11</v>
-      </c>
-      <c r="E57" s="48" t="s">
-        <v>145</v>
-      </c>
-      <c r="F57" s="49"/>
-      <c r="G57" s="50" t="s">
-        <v>7</v>
-      </c>
-      <c r="H57" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="I57" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="J57" s="48" t="s">
-        <v>145</v>
-      </c>
-      <c r="M57" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13">
-      <c r="A58" s="52"/>
-      <c r="B58" s="53"/>
-      <c r="C58" s="53"/>
-      <c r="D58" s="54"/>
-      <c r="E58" s="55"/>
-      <c r="F58" s="56"/>
-      <c r="G58" s="53"/>
-      <c r="H58" s="53"/>
-      <c r="I58" s="57"/>
-      <c r="J58" s="57"/>
-      <c r="M58" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13">
-      <c r="A59" s="58"/>
-      <c r="B59" s="59"/>
-      <c r="C59" s="59"/>
-      <c r="D59" s="60"/>
-      <c r="E59" s="61"/>
-      <c r="F59" s="56"/>
-      <c r="G59" s="59"/>
-      <c r="H59" s="59"/>
-      <c r="I59" s="62"/>
-      <c r="J59" s="62"/>
-      <c r="M59" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13">
-      <c r="A60" s="58"/>
-      <c r="B60" s="59"/>
-      <c r="C60" s="59"/>
-      <c r="D60" s="60"/>
-      <c r="E60" s="61"/>
-      <c r="F60" s="56"/>
-      <c r="G60" s="59"/>
-      <c r="H60" s="59"/>
-      <c r="I60" s="62"/>
-      <c r="J60" s="62"/>
-      <c r="M60" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13">
-      <c r="A61" s="58"/>
-      <c r="B61" s="59"/>
-      <c r="C61" s="59"/>
-      <c r="D61" s="60"/>
-      <c r="E61" s="61"/>
-      <c r="F61" s="56"/>
-      <c r="G61" s="59"/>
-      <c r="H61" s="59"/>
-      <c r="I61" s="62"/>
-      <c r="J61" s="62"/>
-      <c r="M61" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13">
-      <c r="A62" s="58"/>
-      <c r="B62" s="59"/>
-      <c r="C62" s="59"/>
-      <c r="D62" s="60"/>
-      <c r="E62" s="61"/>
-      <c r="F62" s="56"/>
-      <c r="G62" s="59"/>
-      <c r="H62" s="59"/>
-      <c r="I62" s="62"/>
-      <c r="J62" s="62"/>
-      <c r="M62" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13">
-      <c r="A63" s="58"/>
-      <c r="B63" s="59"/>
-      <c r="C63" s="59"/>
-      <c r="D63" s="60"/>
-      <c r="E63" s="61"/>
-      <c r="F63" s="56"/>
-      <c r="G63" s="59"/>
-      <c r="H63" s="59"/>
-      <c r="I63" s="62"/>
-      <c r="J63" s="62"/>
-      <c r="M63" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13">
-      <c r="A64" s="58"/>
-      <c r="B64" s="59"/>
-      <c r="C64" s="59"/>
-      <c r="D64" s="60"/>
-      <c r="E64" s="61"/>
-      <c r="F64" s="56"/>
-      <c r="G64" s="59"/>
-      <c r="H64" s="59"/>
-      <c r="I64" s="62"/>
-      <c r="J64" s="62"/>
-      <c r="M64" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13">
-      <c r="A65" s="58"/>
-      <c r="B65" s="59"/>
-      <c r="C65" s="59"/>
-      <c r="D65" s="60"/>
-      <c r="E65" s="61"/>
-      <c r="F65" s="56"/>
-      <c r="G65" s="59"/>
-      <c r="H65" s="59"/>
-      <c r="I65" s="62"/>
-      <c r="J65" s="62"/>
-      <c r="M65" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13">
-      <c r="A66" s="58"/>
-      <c r="B66" s="59"/>
-      <c r="C66" s="59"/>
-      <c r="D66" s="60"/>
-      <c r="E66" s="61"/>
-      <c r="F66" s="56"/>
-      <c r="G66" s="59"/>
-      <c r="H66" s="59"/>
-      <c r="I66" s="62"/>
-      <c r="J66" s="62"/>
-    </row>
-    <row r="67" spans="1:13">
-      <c r="A67" s="58"/>
-      <c r="B67" s="59"/>
-      <c r="C67" s="59"/>
-      <c r="D67" s="60"/>
-      <c r="E67" s="61"/>
-      <c r="F67" s="56"/>
-      <c r="G67" s="59"/>
-      <c r="H67" s="59"/>
-      <c r="I67" s="62"/>
-      <c r="J67" s="62"/>
-    </row>
-    <row r="68" spans="1:13">
-      <c r="A68" s="58"/>
-      <c r="B68" s="59"/>
-      <c r="C68" s="59"/>
-      <c r="D68" s="60"/>
-      <c r="E68" s="61"/>
-      <c r="F68" s="56"/>
-      <c r="G68" s="59"/>
-      <c r="H68" s="59"/>
-      <c r="I68" s="62"/>
-      <c r="J68" s="62"/>
-      <c r="M68" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13">
-      <c r="A69" s="58"/>
-      <c r="B69" s="59"/>
-      <c r="C69" s="59"/>
-      <c r="D69" s="60"/>
-      <c r="E69" s="61"/>
-      <c r="F69" s="56"/>
-      <c r="G69" s="59"/>
-      <c r="H69" s="59"/>
-      <c r="I69" s="62"/>
-      <c r="J69" s="62"/>
-      <c r="M69" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13">
-      <c r="A70" s="58"/>
-      <c r="B70" s="59"/>
-      <c r="C70" s="59"/>
-      <c r="D70" s="60"/>
-      <c r="E70" s="61"/>
-      <c r="F70" s="56"/>
-      <c r="G70" s="59"/>
-      <c r="H70" s="59"/>
-      <c r="I70" s="62"/>
-      <c r="J70" s="62"/>
-      <c r="M70" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13">
-      <c r="A71" s="58"/>
-      <c r="B71" s="59"/>
-      <c r="C71" s="59"/>
-      <c r="D71" s="60"/>
-      <c r="E71" s="61"/>
-      <c r="F71" s="56"/>
-      <c r="G71" s="59"/>
-      <c r="H71" s="59"/>
-      <c r="I71" s="62"/>
-      <c r="J71" s="62"/>
-    </row>
-    <row r="72" spans="1:13">
-      <c r="A72" s="58"/>
-      <c r="B72" s="59"/>
-      <c r="C72" s="59"/>
-      <c r="D72" s="60"/>
-      <c r="E72" s="61"/>
-      <c r="F72" s="56"/>
-      <c r="G72" s="59"/>
-      <c r="H72" s="59"/>
-      <c r="I72" s="62"/>
-      <c r="J72" s="62"/>
-      <c r="M72" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13">
-      <c r="A73" s="58"/>
-      <c r="B73" s="59"/>
-      <c r="C73" s="59"/>
-      <c r="D73" s="60"/>
-      <c r="E73" s="61"/>
-      <c r="F73" s="56"/>
-      <c r="G73" s="59"/>
-      <c r="H73" s="59"/>
-      <c r="I73" s="62"/>
-      <c r="J73" s="62"/>
-      <c r="M73" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13">
-      <c r="A74" s="58"/>
-      <c r="B74" s="59"/>
-      <c r="C74" s="59"/>
-      <c r="D74" s="60"/>
-      <c r="E74" s="61"/>
-      <c r="F74" s="56"/>
-      <c r="G74" s="59"/>
-      <c r="H74" s="59"/>
-      <c r="I74" s="62"/>
-      <c r="J74" s="62"/>
-      <c r="M74" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13">
-      <c r="A75" s="58"/>
-      <c r="B75" s="59"/>
-      <c r="C75" s="59"/>
-      <c r="D75" s="60"/>
-      <c r="E75" s="61"/>
-      <c r="F75" s="56"/>
-      <c r="G75" s="59"/>
-      <c r="H75" s="59"/>
-      <c r="I75" s="62"/>
-      <c r="J75" s="62"/>
-      <c r="M75" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13">
-      <c r="A76" s="58"/>
-      <c r="B76" s="59"/>
-      <c r="C76" s="59"/>
-      <c r="D76" s="60"/>
-      <c r="E76" s="61"/>
-      <c r="F76" s="56"/>
-      <c r="G76" s="59"/>
-      <c r="H76" s="59"/>
-      <c r="I76" s="62"/>
-      <c r="J76" s="62"/>
-      <c r="M76">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13">
-      <c r="A77" s="58"/>
-      <c r="B77" s="59"/>
-      <c r="C77" s="59"/>
-      <c r="D77" s="60"/>
-      <c r="E77" s="61"/>
-      <c r="F77" s="56"/>
-      <c r="G77" s="59"/>
-      <c r="H77" s="59"/>
-      <c r="I77" s="62"/>
-      <c r="J77" s="62"/>
-    </row>
-    <row r="78" spans="1:13">
-      <c r="A78" s="58"/>
-      <c r="B78" s="59"/>
-      <c r="C78" s="59"/>
-      <c r="D78" s="60"/>
-      <c r="E78" s="61"/>
-      <c r="F78" s="56"/>
-      <c r="G78" s="59"/>
-      <c r="H78" s="59"/>
-      <c r="I78" s="62"/>
-      <c r="J78" s="62"/>
-    </row>
-    <row r="79" spans="1:13">
-      <c r="A79" s="58"/>
-      <c r="B79" s="59"/>
-      <c r="C79" s="59"/>
-      <c r="D79" s="60"/>
-      <c r="E79" s="61"/>
-      <c r="F79" s="56"/>
-      <c r="G79" s="59"/>
-      <c r="H79" s="59"/>
-      <c r="I79" s="62"/>
-      <c r="J79" s="62"/>
-    </row>
-    <row r="80" spans="1:13">
-      <c r="A80" s="58"/>
-      <c r="B80" s="59"/>
-      <c r="C80" s="59"/>
-      <c r="D80" s="60"/>
-      <c r="E80" s="61"/>
-      <c r="F80" s="56"/>
-      <c r="G80" s="59"/>
-      <c r="H80" s="59"/>
-      <c r="I80" s="62"/>
-      <c r="J80" s="62"/>
-    </row>
-    <row r="81" spans="1:12">
-      <c r="A81" s="58"/>
-      <c r="B81" s="59"/>
-      <c r="C81" s="59"/>
-      <c r="D81" s="60"/>
-      <c r="E81" s="61"/>
-      <c r="F81" s="56"/>
-      <c r="G81" s="59"/>
-      <c r="H81" s="59"/>
-      <c r="I81" s="62"/>
-      <c r="J81" s="62"/>
-    </row>
-    <row r="82" spans="1:12" ht="14.7" thickBot="1">
-      <c r="A82" s="63"/>
-      <c r="B82" s="63"/>
-      <c r="C82" s="8"/>
-      <c r="D82" s="64"/>
-      <c r="E82" s="8"/>
-      <c r="F82" s="8"/>
-      <c r="G82" s="63"/>
-      <c r="H82" s="8"/>
-      <c r="I82" s="64"/>
-      <c r="J82" s="8"/>
-    </row>
-    <row r="83" spans="1:12" ht="17.7" thickBot="1">
-      <c r="A83" s="85" t="s">
-        <v>6</v>
-      </c>
-      <c r="B83" s="97"/>
-      <c r="C83" s="86"/>
-      <c r="D83" s="65">
-        <f>SUM($D$58:$D$81)</f>
-        <v>0</v>
-      </c>
-      <c r="E83" s="15"/>
-      <c r="F83" s="15"/>
-      <c r="G83" s="85" t="s">
-        <v>6</v>
-      </c>
-      <c r="H83" s="86"/>
-      <c r="I83" s="65">
-        <f>SUM(I58:I81)</f>
-        <v>0</v>
-      </c>
+      <c r="H83" s="8"/>
+      <c r="I83" s="8"/>
       <c r="J83" s="8"/>
     </row>
-    <row r="84" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A84" s="101" t="s">
-        <v>147</v>
-      </c>
-      <c r="B84" s="102"/>
-      <c r="C84" s="103"/>
-      <c r="D84" s="78">
-        <f>SUMIF($B$58:$B$81,גיליון2!$D$2,גיליון1!$D$58:$D$81)</f>
-        <v>0</v>
-      </c>
+    <row r="84" spans="1:13" ht="14.7" thickBot="1">
+      <c r="A84" s="8"/>
+      <c r="B84" s="8"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
       <c r="E84" s="8"/>
       <c r="F84" s="8"/>
-      <c r="G84" s="63"/>
-      <c r="H84" s="63"/>
+      <c r="G84" s="8"/>
+      <c r="H84" s="8"/>
       <c r="I84" s="8"/>
       <c r="J84" s="8"/>
     </row>
-    <row r="85" spans="1:12" ht="14.7" thickBot="1">
-      <c r="A85" s="98" t="s">
-        <v>148</v>
-      </c>
-      <c r="B85" s="99"/>
-      <c r="C85" s="100"/>
-      <c r="D85" s="78">
-        <f>SUMIF($B$58:$B$81,גיליון2!$D$3,גיליון1!$D$58:$D$81)</f>
+    <row r="85" spans="1:13" s="3" customFormat="1" ht="16" thickBot="1">
+      <c r="A85" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B85" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="C85" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="D85" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="E85" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="F85" s="47"/>
+      <c r="G85" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="H85" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="I85" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="J85" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="M85" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13">
+      <c r="A86" s="50"/>
+      <c r="B86" s="51"/>
+      <c r="C86" s="51"/>
+      <c r="D86" s="52"/>
+      <c r="E86" s="53"/>
+      <c r="F86" s="54"/>
+      <c r="G86" s="51"/>
+      <c r="H86" s="51"/>
+      <c r="I86" s="55"/>
+      <c r="J86" s="55"/>
+      <c r="M86" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13">
+      <c r="A87" s="56"/>
+      <c r="B87" s="57"/>
+      <c r="C87" s="57"/>
+      <c r="D87" s="58"/>
+      <c r="E87" s="59"/>
+      <c r="F87" s="54"/>
+      <c r="G87" s="57"/>
+      <c r="H87" s="57"/>
+      <c r="I87" s="60"/>
+      <c r="J87" s="60"/>
+      <c r="M87" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13">
+      <c r="A88" s="56"/>
+      <c r="B88" s="57"/>
+      <c r="C88" s="57"/>
+      <c r="D88" s="58"/>
+      <c r="E88" s="59"/>
+      <c r="F88" s="54"/>
+      <c r="G88" s="57"/>
+      <c r="H88" s="57"/>
+      <c r="I88" s="60"/>
+      <c r="J88" s="60"/>
+      <c r="M88" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13">
+      <c r="A89" s="56"/>
+      <c r="B89" s="57"/>
+      <c r="C89" s="57"/>
+      <c r="D89" s="58"/>
+      <c r="E89" s="59"/>
+      <c r="F89" s="54"/>
+      <c r="G89" s="57"/>
+      <c r="H89" s="57"/>
+      <c r="I89" s="60"/>
+      <c r="J89" s="60"/>
+      <c r="M89" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13">
+      <c r="A90" s="56"/>
+      <c r="B90" s="57"/>
+      <c r="C90" s="57"/>
+      <c r="D90" s="58"/>
+      <c r="E90" s="59"/>
+      <c r="F90" s="54"/>
+      <c r="G90" s="57"/>
+      <c r="H90" s="57"/>
+      <c r="I90" s="60"/>
+      <c r="J90" s="60"/>
+      <c r="M90" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13">
+      <c r="A91" s="56"/>
+      <c r="B91" s="57"/>
+      <c r="C91" s="57"/>
+      <c r="D91" s="58"/>
+      <c r="E91" s="59"/>
+      <c r="F91" s="54"/>
+      <c r="G91" s="57"/>
+      <c r="H91" s="57"/>
+      <c r="I91" s="60"/>
+      <c r="J91" s="60"/>
+      <c r="M91" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13">
+      <c r="A92" s="56"/>
+      <c r="B92" s="57"/>
+      <c r="C92" s="57"/>
+      <c r="D92" s="58"/>
+      <c r="E92" s="59"/>
+      <c r="F92" s="54"/>
+      <c r="G92" s="57"/>
+      <c r="H92" s="57"/>
+      <c r="I92" s="60"/>
+      <c r="J92" s="60"/>
+      <c r="M92" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13">
+      <c r="A93" s="56"/>
+      <c r="B93" s="57"/>
+      <c r="C93" s="57"/>
+      <c r="D93" s="58"/>
+      <c r="E93" s="59"/>
+      <c r="F93" s="54"/>
+      <c r="G93" s="57"/>
+      <c r="H93" s="57"/>
+      <c r="I93" s="60"/>
+      <c r="J93" s="60"/>
+      <c r="M93" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13">
+      <c r="A94" s="56"/>
+      <c r="B94" s="57"/>
+      <c r="C94" s="57"/>
+      <c r="D94" s="58"/>
+      <c r="E94" s="59"/>
+      <c r="F94" s="54"/>
+      <c r="G94" s="57"/>
+      <c r="H94" s="57"/>
+      <c r="I94" s="60"/>
+      <c r="J94" s="60"/>
+    </row>
+    <row r="95" spans="1:13">
+      <c r="A95" s="56"/>
+      <c r="B95" s="57"/>
+      <c r="C95" s="57"/>
+      <c r="D95" s="58"/>
+      <c r="E95" s="59"/>
+      <c r="F95" s="54"/>
+      <c r="G95" s="57"/>
+      <c r="H95" s="57"/>
+      <c r="I95" s="60"/>
+      <c r="J95" s="60"/>
+    </row>
+    <row r="96" spans="1:13">
+      <c r="A96" s="56"/>
+      <c r="B96" s="57"/>
+      <c r="C96" s="57"/>
+      <c r="D96" s="58"/>
+      <c r="E96" s="59"/>
+      <c r="F96" s="54"/>
+      <c r="G96" s="57"/>
+      <c r="H96" s="57"/>
+      <c r="I96" s="60"/>
+      <c r="J96" s="60"/>
+      <c r="M96" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13">
+      <c r="A97" s="56"/>
+      <c r="B97" s="57"/>
+      <c r="C97" s="57"/>
+      <c r="D97" s="58"/>
+      <c r="E97" s="59"/>
+      <c r="F97" s="54"/>
+      <c r="G97" s="57"/>
+      <c r="H97" s="57"/>
+      <c r="I97" s="60"/>
+      <c r="J97" s="60"/>
+      <c r="M97" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13">
+      <c r="A98" s="56"/>
+      <c r="B98" s="57"/>
+      <c r="C98" s="57"/>
+      <c r="D98" s="58"/>
+      <c r="E98" s="59"/>
+      <c r="F98" s="54"/>
+      <c r="G98" s="57"/>
+      <c r="H98" s="57"/>
+      <c r="I98" s="60"/>
+      <c r="J98" s="60"/>
+      <c r="M98" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13">
+      <c r="A99" s="56"/>
+      <c r="B99" s="57"/>
+      <c r="C99" s="57"/>
+      <c r="D99" s="58"/>
+      <c r="E99" s="59"/>
+      <c r="F99" s="54"/>
+      <c r="G99" s="57"/>
+      <c r="H99" s="57"/>
+      <c r="I99" s="60"/>
+      <c r="J99" s="60"/>
+    </row>
+    <row r="100" spans="1:13">
+      <c r="A100" s="56"/>
+      <c r="B100" s="57"/>
+      <c r="C100" s="57"/>
+      <c r="D100" s="58"/>
+      <c r="E100" s="59"/>
+      <c r="F100" s="54"/>
+      <c r="G100" s="57"/>
+      <c r="H100" s="57"/>
+      <c r="I100" s="60"/>
+      <c r="J100" s="60"/>
+      <c r="M100" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13">
+      <c r="A101" s="56"/>
+      <c r="B101" s="57"/>
+      <c r="C101" s="57"/>
+      <c r="D101" s="58"/>
+      <c r="E101" s="59"/>
+      <c r="F101" s="54"/>
+      <c r="G101" s="57"/>
+      <c r="H101" s="57"/>
+      <c r="I101" s="60"/>
+      <c r="J101" s="60"/>
+      <c r="M101" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13">
+      <c r="A102" s="56"/>
+      <c r="B102" s="57"/>
+      <c r="C102" s="57"/>
+      <c r="D102" s="58"/>
+      <c r="E102" s="59"/>
+      <c r="F102" s="54"/>
+      <c r="G102" s="57"/>
+      <c r="H102" s="57"/>
+      <c r="I102" s="60"/>
+      <c r="J102" s="60"/>
+      <c r="M102" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13">
+      <c r="A103" s="56"/>
+      <c r="B103" s="57"/>
+      <c r="C103" s="57"/>
+      <c r="D103" s="58"/>
+      <c r="E103" s="59"/>
+      <c r="F103" s="54"/>
+      <c r="G103" s="57"/>
+      <c r="H103" s="57"/>
+      <c r="I103" s="60"/>
+      <c r="J103" s="60"/>
+      <c r="M103" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13">
+      <c r="A104" s="56"/>
+      <c r="B104" s="57"/>
+      <c r="C104" s="57"/>
+      <c r="D104" s="58"/>
+      <c r="E104" s="59"/>
+      <c r="F104" s="54"/>
+      <c r="G104" s="57"/>
+      <c r="H104" s="57"/>
+      <c r="I104" s="60"/>
+      <c r="J104" s="60"/>
+      <c r="M104">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13">
+      <c r="A105" s="56"/>
+      <c r="B105" s="57"/>
+      <c r="C105" s="57"/>
+      <c r="D105" s="58"/>
+      <c r="E105" s="59"/>
+      <c r="F105" s="54"/>
+      <c r="G105" s="57"/>
+      <c r="H105" s="57"/>
+      <c r="I105" s="60"/>
+      <c r="J105" s="60"/>
+    </row>
+    <row r="106" spans="1:13">
+      <c r="A106" s="56"/>
+      <c r="B106" s="57"/>
+      <c r="C106" s="57"/>
+      <c r="D106" s="58"/>
+      <c r="E106" s="59"/>
+      <c r="F106" s="54"/>
+      <c r="G106" s="57"/>
+      <c r="H106" s="57"/>
+      <c r="I106" s="60"/>
+      <c r="J106" s="60"/>
+    </row>
+    <row r="107" spans="1:13">
+      <c r="A107" s="56"/>
+      <c r="B107" s="57"/>
+      <c r="C107" s="57"/>
+      <c r="D107" s="58"/>
+      <c r="E107" s="59"/>
+      <c r="F107" s="54"/>
+      <c r="G107" s="57"/>
+      <c r="H107" s="57"/>
+      <c r="I107" s="60"/>
+      <c r="J107" s="60"/>
+    </row>
+    <row r="108" spans="1:13">
+      <c r="A108" s="56"/>
+      <c r="B108" s="57"/>
+      <c r="C108" s="57"/>
+      <c r="D108" s="58"/>
+      <c r="E108" s="59"/>
+      <c r="F108" s="54"/>
+      <c r="G108" s="57"/>
+      <c r="H108" s="57"/>
+      <c r="I108" s="60"/>
+      <c r="J108" s="60"/>
+    </row>
+    <row r="109" spans="1:13">
+      <c r="A109" s="56"/>
+      <c r="B109" s="57"/>
+      <c r="C109" s="57"/>
+      <c r="D109" s="58"/>
+      <c r="E109" s="59"/>
+      <c r="F109" s="54"/>
+      <c r="G109" s="57"/>
+      <c r="H109" s="57"/>
+      <c r="I109" s="60"/>
+      <c r="J109" s="60"/>
+    </row>
+    <row r="110" spans="1:13" ht="14.7" thickBot="1">
+      <c r="A110" s="61"/>
+      <c r="B110" s="61"/>
+      <c r="C110" s="8"/>
+      <c r="D110" s="62"/>
+      <c r="E110" s="8"/>
+      <c r="F110" s="8"/>
+      <c r="G110" s="61"/>
+      <c r="H110" s="8"/>
+      <c r="I110" s="62"/>
+      <c r="J110" s="8"/>
+    </row>
+    <row r="111" spans="1:13" ht="17.7" thickBot="1">
+      <c r="A111" s="88" t="s">
+        <v>6</v>
+      </c>
+      <c r="B111" s="100"/>
+      <c r="C111" s="89"/>
+      <c r="D111" s="63">
+        <f>SUM($D$86:$D$109)</f>
         <v>0</v>
       </c>
-      <c r="E85" s="8"/>
-      <c r="F85" s="8"/>
-      <c r="G85" s="63"/>
-      <c r="H85" s="63"/>
-      <c r="I85" s="8"/>
-      <c r="J85" s="8"/>
-    </row>
-    <row r="86" spans="1:12" ht="17.7" thickBot="1">
-      <c r="A86" s="85" t="s">
-        <v>144</v>
-      </c>
-      <c r="B86" s="97"/>
-      <c r="C86" s="86"/>
-      <c r="D86" s="65">
-        <f>$D$83-$D$84-$D$85</f>
+      <c r="E111" s="15"/>
+      <c r="F111" s="15"/>
+      <c r="G111" s="88" t="s">
+        <v>6</v>
+      </c>
+      <c r="H111" s="89"/>
+      <c r="I111" s="63">
+        <f>SUM(I86:I109)</f>
         <v>0</v>
       </c>
-      <c r="E86" s="8"/>
-      <c r="F86" s="8"/>
-      <c r="G86" s="63"/>
-      <c r="H86" s="63"/>
-      <c r="I86" s="8"/>
-      <c r="J86" s="8"/>
-    </row>
-    <row r="87" spans="1:12" s="73" customFormat="1" ht="17.350000000000001">
-      <c r="A87" s="71"/>
-      <c r="B87" s="71"/>
-      <c r="C87" s="63"/>
-      <c r="D87" s="66"/>
-      <c r="E87" s="72"/>
-      <c r="F87" s="72"/>
-      <c r="G87" s="63"/>
-      <c r="H87" s="63"/>
-      <c r="I87" s="72"/>
-      <c r="J87" s="72"/>
-    </row>
-    <row r="88" spans="1:12" ht="17.25" customHeight="1">
-      <c r="A88" s="69"/>
-      <c r="B88" s="69"/>
-      <c r="C88" s="69"/>
-      <c r="D88" s="69"/>
-      <c r="E88" s="69"/>
-      <c r="F88" s="69"/>
-      <c r="G88" s="69"/>
-      <c r="H88" s="69"/>
-      <c r="I88" s="69"/>
-      <c r="J88" s="69"/>
-      <c r="K88" s="69"/>
-      <c r="L88" s="69"/>
-    </row>
-    <row r="89" spans="1:12" ht="20">
-      <c r="A89" s="81" t="s">
-        <v>152</v>
-      </c>
-      <c r="B89" s="70"/>
-      <c r="C89" s="79" t="s">
-        <v>114</v>
-      </c>
-      <c r="D89" s="79"/>
-      <c r="E89" s="79"/>
-      <c r="F89" s="79"/>
-      <c r="G89" s="79"/>
-      <c r="H89" s="79"/>
-      <c r="I89" s="79"/>
-      <c r="J89" s="79"/>
-      <c r="K89" s="79"/>
-      <c r="L89" s="8"/>
-    </row>
-    <row r="90" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A90" s="87"/>
-      <c r="B90" s="88"/>
-      <c r="C90" s="88"/>
-      <c r="D90" s="88"/>
-      <c r="E90" s="88"/>
-      <c r="F90" s="88"/>
-      <c r="G90" s="88"/>
-      <c r="H90" s="88"/>
-      <c r="I90" s="88"/>
-      <c r="J90" s="88"/>
-      <c r="K90" s="88"/>
-      <c r="L90" s="89"/>
-    </row>
-    <row r="91" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A91" s="90"/>
-      <c r="B91" s="91"/>
-      <c r="C91" s="91"/>
-      <c r="D91" s="91"/>
-      <c r="E91" s="91"/>
-      <c r="F91" s="91"/>
-      <c r="G91" s="91"/>
-      <c r="H91" s="91"/>
-      <c r="I91" s="91"/>
-      <c r="J91" s="91"/>
-      <c r="K91" s="91"/>
-      <c r="L91" s="92"/>
-    </row>
-    <row r="92" spans="1:12">
-      <c r="A92" s="90"/>
-      <c r="B92" s="91"/>
-      <c r="C92" s="91"/>
-      <c r="D92" s="91"/>
-      <c r="E92" s="91"/>
-      <c r="F92" s="91"/>
-      <c r="G92" s="91"/>
-      <c r="H92" s="91"/>
-      <c r="I92" s="91"/>
-      <c r="J92" s="91"/>
-      <c r="K92" s="91"/>
-      <c r="L92" s="92"/>
-    </row>
-    <row r="93" spans="1:12">
-      <c r="A93" s="90"/>
-      <c r="B93" s="91"/>
-      <c r="C93" s="91"/>
-      <c r="D93" s="91"/>
-      <c r="E93" s="91"/>
-      <c r="F93" s="91"/>
-      <c r="G93" s="91"/>
-      <c r="H93" s="91"/>
-      <c r="I93" s="91"/>
-      <c r="J93" s="91"/>
-      <c r="K93" s="91"/>
-      <c r="L93" s="92"/>
-    </row>
-    <row r="94" spans="1:12">
-      <c r="A94" s="93"/>
-      <c r="B94" s="94"/>
-      <c r="C94" s="94"/>
-      <c r="D94" s="94"/>
-      <c r="E94" s="94"/>
-      <c r="F94" s="94"/>
-      <c r="G94" s="94"/>
-      <c r="H94" s="94"/>
-      <c r="I94" s="94"/>
-      <c r="J94" s="94"/>
-      <c r="K94" s="94"/>
-      <c r="L94" s="95"/>
-    </row>
-    <row r="95" spans="1:12">
-      <c r="A95" s="8"/>
-      <c r="B95" s="8"/>
-      <c r="C95" s="8"/>
-      <c r="D95" s="8"/>
-      <c r="E95" s="8"/>
-      <c r="F95" s="8"/>
-      <c r="G95" s="8"/>
-      <c r="H95" s="8"/>
-      <c r="I95" s="8"/>
-      <c r="J95" s="8"/>
-      <c r="K95" s="8"/>
-      <c r="L95" s="8"/>
+      <c r="J111" s="8"/>
+    </row>
+    <row r="112" spans="1:13" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A112" s="104" t="s">
+        <v>41</v>
+      </c>
+      <c r="B112" s="105"/>
+      <c r="C112" s="106"/>
+      <c r="D112" s="76">
+        <f>SUMIF($B$86:$B$109,#REF!,גיליון1!$D$86:$D$109)</f>
+        <v>0</v>
+      </c>
+      <c r="E112" s="8"/>
+      <c r="F112" s="8"/>
+      <c r="G112" s="61"/>
+      <c r="H112" s="61"/>
+      <c r="I112" s="8"/>
+      <c r="J112" s="8"/>
+    </row>
+    <row r="113" spans="1:12" ht="14.7" thickBot="1">
+      <c r="A113" s="101" t="s">
+        <v>42</v>
+      </c>
+      <c r="B113" s="102"/>
+      <c r="C113" s="103"/>
+      <c r="D113" s="76">
+        <f>SUMIF($B$86:$B$109,#REF!,גיליון1!$D$86:$D$109)</f>
+        <v>0</v>
+      </c>
+      <c r="E113" s="8"/>
+      <c r="F113" s="8"/>
+      <c r="G113" s="61"/>
+      <c r="H113" s="61"/>
+      <c r="I113" s="8"/>
+      <c r="J113" s="8"/>
+    </row>
+    <row r="114" spans="1:12" ht="17.7" thickBot="1">
+      <c r="A114" s="88" t="s">
+        <v>38</v>
+      </c>
+      <c r="B114" s="100"/>
+      <c r="C114" s="89"/>
+      <c r="D114" s="63">
+        <f>$D$111-$D$112-$D$113</f>
+        <v>0</v>
+      </c>
+      <c r="E114" s="8"/>
+      <c r="F114" s="8"/>
+      <c r="G114" s="61"/>
+      <c r="H114" s="61"/>
+      <c r="I114" s="8"/>
+      <c r="J114" s="8"/>
+    </row>
+    <row r="115" spans="1:12" s="71" customFormat="1" ht="17.350000000000001">
+      <c r="A115" s="69"/>
+      <c r="B115" s="69"/>
+      <c r="C115" s="61"/>
+      <c r="D115" s="64"/>
+      <c r="E115" s="70"/>
+      <c r="F115" s="70"/>
+      <c r="G115" s="61"/>
+      <c r="H115" s="61"/>
+      <c r="I115" s="70"/>
+      <c r="J115" s="70"/>
+    </row>
+    <row r="116" spans="1:12" ht="17.25" customHeight="1">
+      <c r="A116" s="67"/>
+      <c r="B116" s="67"/>
+      <c r="C116" s="67"/>
+      <c r="D116" s="67"/>
+      <c r="E116" s="67"/>
+      <c r="F116" s="67"/>
+      <c r="G116" s="67"/>
+      <c r="H116" s="67"/>
+      <c r="I116" s="67"/>
+      <c r="J116" s="67"/>
+      <c r="K116" s="67"/>
+      <c r="L116" s="67"/>
+    </row>
+    <row r="117" spans="1:12" ht="20">
+      <c r="A117" s="79" t="s">
+        <v>43</v>
+      </c>
+      <c r="B117" s="68"/>
+      <c r="C117" s="77" t="s">
+        <v>32</v>
+      </c>
+      <c r="D117" s="77"/>
+      <c r="E117" s="77"/>
+      <c r="F117" s="77"/>
+      <c r="G117" s="77"/>
+      <c r="H117" s="77"/>
+      <c r="I117" s="77"/>
+      <c r="J117" s="77"/>
+      <c r="K117" s="77"/>
+      <c r="L117" s="8"/>
+    </row>
+    <row r="118" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A118" s="90"/>
+      <c r="B118" s="91"/>
+      <c r="C118" s="91"/>
+      <c r="D118" s="91"/>
+      <c r="E118" s="91"/>
+      <c r="F118" s="91"/>
+      <c r="G118" s="91"/>
+      <c r="H118" s="91"/>
+      <c r="I118" s="91"/>
+      <c r="J118" s="91"/>
+      <c r="K118" s="91"/>
+      <c r="L118" s="92"/>
+    </row>
+    <row r="119" spans="1:12" ht="16.5" customHeight="1">
+      <c r="A119" s="93"/>
+      <c r="B119" s="94"/>
+      <c r="C119" s="94"/>
+      <c r="D119" s="94"/>
+      <c r="E119" s="94"/>
+      <c r="F119" s="94"/>
+      <c r="G119" s="94"/>
+      <c r="H119" s="94"/>
+      <c r="I119" s="94"/>
+      <c r="J119" s="94"/>
+      <c r="K119" s="94"/>
+      <c r="L119" s="95"/>
+    </row>
+    <row r="120" spans="1:12">
+      <c r="A120" s="93"/>
+      <c r="B120" s="94"/>
+      <c r="C120" s="94"/>
+      <c r="D120" s="94"/>
+      <c r="E120" s="94"/>
+      <c r="F120" s="94"/>
+      <c r="G120" s="94"/>
+      <c r="H120" s="94"/>
+      <c r="I120" s="94"/>
+      <c r="J120" s="94"/>
+      <c r="K120" s="94"/>
+      <c r="L120" s="95"/>
+    </row>
+    <row r="121" spans="1:12">
+      <c r="A121" s="93"/>
+      <c r="B121" s="94"/>
+      <c r="C121" s="94"/>
+      <c r="D121" s="94"/>
+      <c r="E121" s="94"/>
+      <c r="F121" s="94"/>
+      <c r="G121" s="94"/>
+      <c r="H121" s="94"/>
+      <c r="I121" s="94"/>
+      <c r="J121" s="94"/>
+      <c r="K121" s="94"/>
+      <c r="L121" s="95"/>
+    </row>
+    <row r="122" spans="1:12">
+      <c r="A122" s="96"/>
+      <c r="B122" s="97"/>
+      <c r="C122" s="97"/>
+      <c r="D122" s="97"/>
+      <c r="E122" s="97"/>
+      <c r="F122" s="97"/>
+      <c r="G122" s="97"/>
+      <c r="H122" s="97"/>
+      <c r="I122" s="97"/>
+      <c r="J122" s="97"/>
+      <c r="K122" s="97"/>
+      <c r="L122" s="98"/>
+    </row>
+    <row r="123" spans="1:12">
+      <c r="A123" s="8"/>
+      <c r="B123" s="8"/>
+      <c r="C123" s="8"/>
+      <c r="D123" s="8"/>
+      <c r="E123" s="8"/>
+      <c r="F123" s="8"/>
+      <c r="G123" s="8"/>
+      <c r="H123" s="8"/>
+      <c r="I123" s="8"/>
+      <c r="J123" s="8"/>
+      <c r="K123" s="8"/>
+      <c r="L123" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="A4:K6"/>
-    <mergeCell ref="G83:H83"/>
-    <mergeCell ref="A90:L94"/>
-    <mergeCell ref="A53:K53"/>
-    <mergeCell ref="A83:C83"/>
-    <mergeCell ref="A86:C86"/>
-    <mergeCell ref="A85:C85"/>
-    <mergeCell ref="A84:C84"/>
-    <mergeCell ref="A51:K51"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="G111:H111"/>
+    <mergeCell ref="A118:L122"/>
+    <mergeCell ref="A81:K81"/>
+    <mergeCell ref="A111:C111"/>
+    <mergeCell ref="A114:C114"/>
+    <mergeCell ref="A113:C113"/>
+    <mergeCell ref="A112:C112"/>
+    <mergeCell ref="A79:K79"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A62:D62"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B58:B81 B45:B48 B18:B33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B86:B109 B73:B76 B18:B57">
       <formula1>INDIRECT($A18)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H58:H81">
-      <formula1>INDIRECT($G58)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H86:H109">
+      <formula1>INDIRECT($G86)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G58:G81 F45:F48">
-      <formula1>$M$68:$M$76</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G86:G109 F73:F76">
+      <formula1>$M$96:$M$104</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A58:A81 A45:A48 A18:A33">
-      <formula1>$M$57:$M$65</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A86:A109 A18:A57 A73:A76">
+      <formula1>$M$85:$M$93</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G45:G48">
-      <formula1>INDIRECT($F45)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G73:G76">
+      <formula1>INDIRECT($F73)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC43"/>
-  <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35"/>
-  <cols>
-    <col min="1" max="1" width="15.64453125" customWidth="1"/>
-    <col min="2" max="13" width="9" customWidth="1"/>
-    <col min="14" max="14" width="22.1171875" customWidth="1"/>
-    <col min="15" max="23" width="9" customWidth="1"/>
-    <col min="24" max="24" width="16.234375" customWidth="1"/>
-    <col min="25" max="26" width="9" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29">
-      <c r="N1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J2" t="s">
-        <v>62</v>
-      </c>
-      <c r="L2" t="s">
-        <v>65</v>
-      </c>
-      <c r="N2" t="s">
-        <v>68</v>
-      </c>
-      <c r="O2" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>85</v>
-      </c>
-      <c r="S2" t="s">
-        <v>85</v>
-      </c>
-      <c r="U2" t="s">
-        <v>92</v>
-      </c>
-      <c r="X2" t="s">
-        <v>97</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>106</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" t="s">
-        <v>57</v>
-      </c>
-      <c r="J3" t="s">
-        <v>130</v>
-      </c>
-      <c r="L3" t="s">
-        <v>66</v>
-      </c>
-      <c r="N3" t="s">
-        <v>112</v>
-      </c>
-      <c r="O3" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>86</v>
-      </c>
-      <c r="S3" t="s">
-        <v>86</v>
-      </c>
-      <c r="U3" t="s">
-        <v>94</v>
-      </c>
-      <c r="X3" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>101</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29">
-      <c r="A4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>51</v>
-      </c>
-      <c r="H4" t="s">
-        <v>58</v>
-      </c>
-      <c r="J4" t="s">
-        <v>64</v>
-      </c>
-      <c r="L4" t="s">
-        <v>67</v>
-      </c>
-      <c r="N4" t="s">
-        <v>111</v>
-      </c>
-      <c r="O4" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>87</v>
-      </c>
-      <c r="S4" t="s">
-        <v>87</v>
-      </c>
-      <c r="U4" t="s">
-        <v>95</v>
-      </c>
-      <c r="X4" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>102</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>107</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H5" t="s">
-        <v>59</v>
-      </c>
-      <c r="J5" t="s">
-        <v>63</v>
-      </c>
-      <c r="N5" t="s">
-        <v>69</v>
-      </c>
-      <c r="O5" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>88</v>
-      </c>
-      <c r="S5" t="s">
-        <v>89</v>
-      </c>
-      <c r="U5" t="s">
-        <v>96</v>
-      </c>
-      <c r="X5" t="s">
-        <v>154</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>108</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" t="s">
-        <v>126</v>
-      </c>
-      <c r="H6" t="s">
-        <v>60</v>
-      </c>
-      <c r="N6" t="s">
-        <v>115</v>
-      </c>
-      <c r="O6" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>91</v>
-      </c>
-      <c r="S6" t="s">
-        <v>90</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>109</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H7" t="s">
-        <v>61</v>
-      </c>
-      <c r="N7" t="s">
-        <v>72</v>
-      </c>
-      <c r="O7" t="s">
-        <v>157</v>
-      </c>
-      <c r="S7" t="s">
-        <v>91</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29">
-      <c r="A8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" t="s">
-        <v>54</v>
-      </c>
-      <c r="N8" t="s">
-        <v>73</v>
-      </c>
-      <c r="S8" t="s">
-        <v>129</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29">
-      <c r="A9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" t="s">
-        <v>133</v>
-      </c>
-      <c r="F9" t="s">
-        <v>55</v>
-      </c>
-      <c r="N9" t="s">
-        <v>74</v>
-      </c>
-      <c r="S9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29">
-      <c r="A10" t="s">
-        <v>155</v>
-      </c>
-      <c r="D10" t="s">
-        <v>132</v>
-      </c>
-      <c r="N10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29">
-      <c r="D11" t="s">
-        <v>134</v>
-      </c>
-      <c r="N11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29">
-      <c r="A12" t="s">
-        <v>122</v>
-      </c>
-      <c r="D12" t="s">
-        <v>135</v>
-      </c>
-      <c r="N12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29">
-      <c r="D13" t="s">
-        <v>153</v>
-      </c>
-      <c r="N13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29">
-      <c r="A14" t="s">
-        <v>123</v>
-      </c>
-      <c r="D14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29">
-      <c r="A15" t="s">
-        <v>124</v>
-      </c>
-      <c r="D15" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="16" spans="1:29">
-      <c r="D16" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>116</v>
-      </c>
-      <c r="D17" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>81</v>
-      </c>
-      <c r="D18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="D19" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>105</v>
-      </c>
-      <c r="D20" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22">
-        <v>562</v>
-      </c>
-      <c r="D22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="D23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="D24" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="D25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="D26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="D27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="D28" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="D29" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="D30" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="D31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="D32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4">
-      <c r="D33" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="4:4">
-      <c r="D34" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="4:4">
-      <c r="D35" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="36" spans="4:4">
-      <c r="D36" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="37" spans="4:4">
-      <c r="D37" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="4:4">
-      <c r="D38" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="39" spans="4:4">
-      <c r="D39" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="40" spans="4:4">
-      <c r="D40" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="4:4">
-      <c r="D41" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="4:4">
-      <c r="D42" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="4:4">
-      <c r="D43" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="0" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>